<commit_message>
changed wealth tax parameters, about to rerun tax experiments
</commit_message>
<xml_diff>
--- a/Data/Effective Wealth Tax Rates.xlsx
+++ b/Data/Effective Wealth Tax Rates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emag42\GIT_REPOS\piketty-wealth-tax\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emag42\GIT_REPOS\wealthtax\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -360,103 +360,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-327671.25376200001</c:v>
+                  <c:v>-463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-245753.44032150001</c:v>
+                  <c:v>-347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-163835.626881</c:v>
+                  <c:v>-231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-81917.813440500002</c:v>
+                  <c:v>-115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81917.813440500002</c:v>
+                  <c:v>115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163835.626881</c:v>
+                  <c:v>231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>245753.44032150001</c:v>
+                  <c:v>347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>327671.25376200001</c:v>
+                  <c:v>463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>409589.06720250001</c:v>
+                  <c:v>579840.07354999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>491506.88064300001</c:v>
+                  <c:v>695808.08825999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>573424.69408349996</c:v>
+                  <c:v>811776.10297000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>655342.50752400002</c:v>
+                  <c:v>927744.11768000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>737260.32096450008</c:v>
+                  <c:v>1043712.13239</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>819178.13440500002</c:v>
+                  <c:v>1159680.1470999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>901095.94784549996</c:v>
+                  <c:v>1275648.16181</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>983013.76128600002</c:v>
+                  <c:v>1391616.17652</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1064931.5747265001</c:v>
+                  <c:v>1507584.19123</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1146849.3881669999</c:v>
+                  <c:v>1623552.20594</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1228767.2016075</c:v>
+                  <c:v>1739520.22065</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1310685.015048</c:v>
+                  <c:v>1855488.23536</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1392602.8284885001</c:v>
+                  <c:v>1971456.2500700001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1474520.6419290002</c:v>
+                  <c:v>2087424.2647800001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1556438.4553695</c:v>
+                  <c:v>2203392.2794900001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1638356.26881</c:v>
+                  <c:v>2319360.2941999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1720274.0822505001</c:v>
+                  <c:v>2435328.3089100001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1802191.8956909999</c:v>
+                  <c:v>2551296.3236199999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1884109.7091315</c:v>
+                  <c:v>2667264.3383300002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1966027.522572</c:v>
+                  <c:v>2783232.35304</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2047945.3360125001</c:v>
+                  <c:v>2899200.3677500002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2129863.1494530002</c:v>
+                  <c:v>3015168.38246</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2211780.9628935</c:v>
+                  <c:v>3131136.3971700002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2293698.7763339998</c:v>
+                  <c:v>3247104.41188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -483,88 +483,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.3972830989308099E-3</c:v>
+                  <c:v>9.9873995490428573E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.018763801755296E-2</c:v>
+                  <c:v>1.4272852052126977E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2694846923443645E-2</c:v>
+                  <c:v>1.6654993044984981E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4476160651179501E-2</c:v>
+                  <c:v>1.8171397423826743E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5806959904178033E-2</c:v>
+                  <c:v>1.9221442138250947E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.683896866490299E-2</c:v>
+                  <c:v>1.9991592636924165E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.7662657231337399E-2</c:v>
+                  <c:v>2.058059847073759E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8335319864429333E-2</c:v>
+                  <c:v>2.1045644232259391E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.889500504113676E-2</c:v>
+                  <c:v>2.1422136449261449E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9367970489955113E-2</c:v>
+                  <c:v>2.1733169712283833E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.9772922055468628E-2</c:v>
+                  <c:v>2.1994450207187485E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.0123546543139956E-2</c:v>
+                  <c:v>2.2217031522148493E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0430089248805482E-2</c:v>
+                  <c:v>2.2408918642781106E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0700371680509724E-2</c:v>
+                  <c:v>2.2576051172244024E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0940468295190761E-2</c:v>
+                  <c:v>2.2722929085094684E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1155168488186701E-2</c:v>
+                  <c:v>2.2853023975626014E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1348299344761672E-2</c:v>
+                  <c:v>2.2969056951100117E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1522955770740961E-2</c:v>
+                  <c:v>2.3073191033199707E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.168166759641852E-2</c:v>
+                  <c:v>2.3167167255522449E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.182652291289728E-2</c:v>
+                  <c:v>2.3252402785950189E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.1959260455574395E-2</c:v>
+                  <c:v>2.333006288672055E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2081339733614209E-2</c:v>
+                  <c:v>2.3401114504179883E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2193994918170791E-2</c:v>
+                  <c:v>2.3466366736204426E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2298276714465499E-2</c:v>
+                  <c:v>2.3526501779052925E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2395085231668582E-2</c:v>
+                  <c:v>2.3582098868218555E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.2485196030450967E-2</c:v>
+                  <c:v>2.3633652996421256E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.2569280944984765E-2</c:v>
+                  <c:v>2.3681589691406196E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.2647924862871531E-2</c:v>
+                  <c:v>2.3726276788409606E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,11 +579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="285380600"/>
-        <c:axId val="285380992"/>
+        <c:axId val="243999144"/>
+        <c:axId val="243999536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="285380600"/>
+        <c:axId val="243999144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,12 +640,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285380992"/>
+        <c:crossAx val="243999536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="285380992"/>
+        <c:axId val="243999536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285380600"/>
+        <c:crossAx val="243999144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -861,103 +861,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-327671.25376200001</c:v>
+                  <c:v>-463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-245753.44032150001</c:v>
+                  <c:v>-347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-163835.626881</c:v>
+                  <c:v>-231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-81917.813440500002</c:v>
+                  <c:v>-115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81917.813440500002</c:v>
+                  <c:v>115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163835.626881</c:v>
+                  <c:v>231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>245753.44032150001</c:v>
+                  <c:v>347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>327671.25376200001</c:v>
+                  <c:v>463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>409589.06720250001</c:v>
+                  <c:v>579840.07354999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>491506.88064300001</c:v>
+                  <c:v>695808.08825999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>573424.69408349996</c:v>
+                  <c:v>811776.10297000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>655342.50752400002</c:v>
+                  <c:v>927744.11768000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>737260.32096450008</c:v>
+                  <c:v>1043712.13239</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>819178.13440500002</c:v>
+                  <c:v>1159680.1470999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>901095.94784549996</c:v>
+                  <c:v>1275648.16181</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>983013.76128600002</c:v>
+                  <c:v>1391616.17652</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1064931.5747265001</c:v>
+                  <c:v>1507584.19123</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1146849.3881669999</c:v>
+                  <c:v>1623552.20594</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1228767.2016075</c:v>
+                  <c:v>1739520.22065</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1310685.015048</c:v>
+                  <c:v>1855488.23536</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1392602.8284885001</c:v>
+                  <c:v>1971456.2500700001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1474520.6419290002</c:v>
+                  <c:v>2087424.2647800001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1556438.4553695</c:v>
+                  <c:v>2203392.2794900001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1638356.26881</c:v>
+                  <c:v>2319360.2941999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1720274.0822505001</c:v>
+                  <c:v>2435328.3089100001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1802191.8956909999</c:v>
+                  <c:v>2551296.3236199999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1884109.7091315</c:v>
+                  <c:v>2667264.3383300002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1966027.522572</c:v>
+                  <c:v>2783232.35304</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2047945.3360125001</c:v>
+                  <c:v>2899200.3677500002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2129863.1494530002</c:v>
+                  <c:v>3015168.38246</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2211780.9628935</c:v>
+                  <c:v>3131136.3971700002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2293698.7763339998</c:v>
+                  <c:v>3247104.41188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,88 +984,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1157556955946986E-2</c:v>
+                  <c:v>1.5984873107996855E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6223757300038305E-2</c:v>
+                  <c:v>2.039713187617774E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8943328310500624E-2</c:v>
+                  <c:v>2.2214434356830043E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0569952214408695E-2</c:v>
+                  <c:v>2.3134807474267202E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1619520551864387E-2</c:v>
+                  <c:v>2.3664330761536727E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2335902701902593E-2</c:v>
+                  <c:v>2.3996634227419517E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.2846536043806185E-2</c:v>
+                  <c:v>2.4218755604926128E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3223281547621193E-2</c:v>
+                  <c:v>2.4374522818485466E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3509161462090186E-2</c:v>
+                  <c:v>2.4487955696491863E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3731209743919346E-2</c:v>
+                  <c:v>2.4573112794850409E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3907106246471747E-2</c:v>
+                  <c:v>2.4638666817716984E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.404880806732311E-2</c:v>
+                  <c:v>2.4690203458051403E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.416463662904467E-2</c:v>
+                  <c:v>2.4731451896010916E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4260527852569488E-2</c:v>
+                  <c:v>2.4764978883216826E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4340808093505938E-2</c:v>
+                  <c:v>2.4792597921939694E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4408690825830699E-2</c:v>
+                  <c:v>2.4815619758030535E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4466603292981282E-2</c:v>
+                  <c:v>2.483501081328501E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4516406537111061E-2</c:v>
+                  <c:v>2.4851496288218318E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.4559546802373645E-2</c:v>
+                  <c:v>2.4865628965230833E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4597161727105361E-2</c:v>
+                  <c:v>2.4877836159097812E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4630156120918657E-2</c:v>
+                  <c:v>2.4888452401507683E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4659256889976829E-2</c:v>
+                  <c:v>2.4897742606850248E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4685053419229951E-2</c:v>
+                  <c:v>2.4905918760487197E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4708027651536024E-2</c:v>
+                  <c:v>2.4913152119714635E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4728576761989158E-2</c:v>
+                  <c:v>2.4919582255219713E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4747030439789621E-2</c:v>
+                  <c:v>2.4925323834632456E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.4763664195023436E-2</c:v>
+                  <c:v>2.4930471770327742E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4778709701972084E-2</c:v>
+                  <c:v>2.4935105167210238E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,11 +1080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="247515624"/>
-        <c:axId val="76468424"/>
+        <c:axId val="244000320"/>
+        <c:axId val="244000712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="247515624"/>
+        <c:axId val="244000320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,12 +1141,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76468424"/>
+        <c:crossAx val="244000712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76468424"/>
+        <c:axId val="244000712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247515624"/>
+        <c:crossAx val="244000320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1300,103 +1300,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-327671.25376200001</c:v>
+                  <c:v>-463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-245753.44032150001</c:v>
+                  <c:v>-347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-163835.626881</c:v>
+                  <c:v>-231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-81917.813440500002</c:v>
+                  <c:v>-115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81917.813440500002</c:v>
+                  <c:v>115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163835.626881</c:v>
+                  <c:v>231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>245753.44032150001</c:v>
+                  <c:v>347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>327671.25376200001</c:v>
+                  <c:v>463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>409589.06720250001</c:v>
+                  <c:v>579840.07354999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>491506.88064300001</c:v>
+                  <c:v>695808.08825999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>573424.69408349996</c:v>
+                  <c:v>811776.10297000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>655342.50752400002</c:v>
+                  <c:v>927744.11768000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>737260.32096450008</c:v>
+                  <c:v>1043712.13239</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>819178.13440500002</c:v>
+                  <c:v>1159680.1470999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>901095.94784549996</c:v>
+                  <c:v>1275648.16181</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>983013.76128600002</c:v>
+                  <c:v>1391616.17652</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1064931.5747265001</c:v>
+                  <c:v>1507584.19123</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1146849.3881669999</c:v>
+                  <c:v>1623552.20594</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1228767.2016075</c:v>
+                  <c:v>1739520.22065</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1310685.015048</c:v>
+                  <c:v>1855488.23536</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1392602.8284885001</c:v>
+                  <c:v>1971456.2500700001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1474520.6419290002</c:v>
+                  <c:v>2087424.2647800001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1556438.4553695</c:v>
+                  <c:v>2203392.2794900001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1638356.26881</c:v>
+                  <c:v>2319360.2941999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1720274.0822505001</c:v>
+                  <c:v>2435328.3089100001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1802191.8956909999</c:v>
+                  <c:v>2551296.3236199999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1884109.7091315</c:v>
+                  <c:v>2667264.3383300002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1966027.522572</c:v>
+                  <c:v>2783232.35304</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2047945.3360125001</c:v>
+                  <c:v>2899200.3677500002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2129863.1494530002</c:v>
+                  <c:v>3015168.38246</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2211780.9628935</c:v>
+                  <c:v>3131136.3971700002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2293698.7763339998</c:v>
+                  <c:v>3247104.41188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1423,88 +1423,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.3972830989308099E-3</c:v>
+                  <c:v>9.9873995490428573E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.018763801755296E-2</c:v>
+                  <c:v>1.4272852052126977E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2694846923443645E-2</c:v>
+                  <c:v>1.6654993044984981E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4476160651179501E-2</c:v>
+                  <c:v>1.8171397423826743E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5806959904178033E-2</c:v>
+                  <c:v>1.9221442138250947E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.683896866490299E-2</c:v>
+                  <c:v>1.9991592636924165E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.7662657231337399E-2</c:v>
+                  <c:v>2.058059847073759E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8335319864429333E-2</c:v>
+                  <c:v>2.1045644232259391E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.889500504113676E-2</c:v>
+                  <c:v>2.1422136449261449E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9367970489955113E-2</c:v>
+                  <c:v>2.1733169712283833E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.9772922055468628E-2</c:v>
+                  <c:v>2.1994450207187485E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.0123546543139956E-2</c:v>
+                  <c:v>2.2217031522148493E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0430089248805482E-2</c:v>
+                  <c:v>2.2408918642781106E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0700371680509724E-2</c:v>
+                  <c:v>2.2576051172244024E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0940468295190761E-2</c:v>
+                  <c:v>2.2722929085094684E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1155168488186701E-2</c:v>
+                  <c:v>2.2853023975626014E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1348299344761672E-2</c:v>
+                  <c:v>2.2969056951100117E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1522955770740961E-2</c:v>
+                  <c:v>2.3073191033199707E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.168166759641852E-2</c:v>
+                  <c:v>2.3167167255522449E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.182652291289728E-2</c:v>
+                  <c:v>2.3252402785950189E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.1959260455574395E-2</c:v>
+                  <c:v>2.333006288672055E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2081339733614209E-2</c:v>
+                  <c:v>2.3401114504179883E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2193994918170791E-2</c:v>
+                  <c:v>2.3466366736204426E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2298276714465499E-2</c:v>
+                  <c:v>2.3526501779052925E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2395085231668582E-2</c:v>
+                  <c:v>2.3582098868218555E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.2485196030450967E-2</c:v>
+                  <c:v>2.3633652996421256E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.2569280944984765E-2</c:v>
+                  <c:v>2.3681589691406196E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.2647924862871531E-2</c:v>
+                  <c:v>2.3726276788409606E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1547,103 +1547,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-327671.25376200001</c:v>
+                  <c:v>-463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-245753.44032150001</c:v>
+                  <c:v>-347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-163835.626881</c:v>
+                  <c:v>-231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-81917.813440500002</c:v>
+                  <c:v>-115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81917.813440500002</c:v>
+                  <c:v>115968.01471</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163835.626881</c:v>
+                  <c:v>231936.02942000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>245753.44032150001</c:v>
+                  <c:v>347904.04412999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>327671.25376200001</c:v>
+                  <c:v>463872.05884000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>409589.06720250001</c:v>
+                  <c:v>579840.07354999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>491506.88064300001</c:v>
+                  <c:v>695808.08825999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>573424.69408349996</c:v>
+                  <c:v>811776.10297000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>655342.50752400002</c:v>
+                  <c:v>927744.11768000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>737260.32096450008</c:v>
+                  <c:v>1043712.13239</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>819178.13440500002</c:v>
+                  <c:v>1159680.1470999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>901095.94784549996</c:v>
+                  <c:v>1275648.16181</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>983013.76128600002</c:v>
+                  <c:v>1391616.17652</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1064931.5747265001</c:v>
+                  <c:v>1507584.19123</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1146849.3881669999</c:v>
+                  <c:v>1623552.20594</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1228767.2016075</c:v>
+                  <c:v>1739520.22065</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1310685.015048</c:v>
+                  <c:v>1855488.23536</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1392602.8284885001</c:v>
+                  <c:v>1971456.2500700001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1474520.6419290002</c:v>
+                  <c:v>2087424.2647800001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1556438.4553695</c:v>
+                  <c:v>2203392.2794900001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1638356.26881</c:v>
+                  <c:v>2319360.2941999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1720274.0822505001</c:v>
+                  <c:v>2435328.3089100001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1802191.8956909999</c:v>
+                  <c:v>2551296.3236199999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1884109.7091315</c:v>
+                  <c:v>2667264.3383300002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1966027.522572</c:v>
+                  <c:v>2783232.35304</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2047945.3360125001</c:v>
+                  <c:v>2899200.3677500002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2129863.1494530002</c:v>
+                  <c:v>3015168.38246</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2211780.9628935</c:v>
+                  <c:v>3131136.3971700002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2293698.7763339998</c:v>
+                  <c:v>3247104.41188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,88 +1670,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1157556955946986E-2</c:v>
+                  <c:v>1.5984873107996855E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6223757300038305E-2</c:v>
+                  <c:v>2.039713187617774E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8943328310500624E-2</c:v>
+                  <c:v>2.2214434356830043E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0569952214408695E-2</c:v>
+                  <c:v>2.3134807474267202E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1619520551864387E-2</c:v>
+                  <c:v>2.3664330761536727E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2335902701902593E-2</c:v>
+                  <c:v>2.3996634227419517E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.2846536043806185E-2</c:v>
+                  <c:v>2.4218755604926128E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3223281547621193E-2</c:v>
+                  <c:v>2.4374522818485466E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3509161462090186E-2</c:v>
+                  <c:v>2.4487955696491863E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3731209743919346E-2</c:v>
+                  <c:v>2.4573112794850409E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3907106246471747E-2</c:v>
+                  <c:v>2.4638666817716984E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.404880806732311E-2</c:v>
+                  <c:v>2.4690203458051403E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.416463662904467E-2</c:v>
+                  <c:v>2.4731451896010916E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4260527852569488E-2</c:v>
+                  <c:v>2.4764978883216826E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4340808093505938E-2</c:v>
+                  <c:v>2.4792597921939694E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4408690825830699E-2</c:v>
+                  <c:v>2.4815619758030535E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4466603292981282E-2</c:v>
+                  <c:v>2.483501081328501E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4516406537111061E-2</c:v>
+                  <c:v>2.4851496288218318E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.4559546802373645E-2</c:v>
+                  <c:v>2.4865628965230833E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4597161727105361E-2</c:v>
+                  <c:v>2.4877836159097812E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4630156120918657E-2</c:v>
+                  <c:v>2.4888452401507683E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4659256889976829E-2</c:v>
+                  <c:v>2.4897742606850248E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4685053419229951E-2</c:v>
+                  <c:v>2.4905918760487197E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4708027651536024E-2</c:v>
+                  <c:v>2.4913152119714635E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4728576761989158E-2</c:v>
+                  <c:v>2.4919582255219713E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4747030439789621E-2</c:v>
+                  <c:v>2.4925323834632456E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.4763664195023436E-2</c:v>
+                  <c:v>2.4930471770327742E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4778709701972084E-2</c:v>
+                  <c:v>2.4935105167210238E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1766,11 +1766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76469208"/>
-        <c:axId val="76469600"/>
+        <c:axId val="244919936"/>
+        <c:axId val="244920328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76469208"/>
+        <c:axId val="244919936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,12 +1827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76469600"/>
+        <c:crossAx val="244920328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76469600"/>
+        <c:axId val="244920328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,7 +1889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76469208"/>
+        <c:crossAx val="244919936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.01"/>
@@ -4017,7 +4017,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4047,7 +4047,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.0671931633502476</v>
+        <v>1.36350750271454</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E34" si="0">f*D2</f>
-        <v>-327671.25376200001</v>
+        <v>-463872.05884000001</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F37" si="1">IF(D2-bmin&gt;0,p*(h*D2-bmin)/(h*D2-bmin+m),0)</f>
@@ -4073,7 +4073,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.551650285718883</v>
+        <v>1.02478093770152</v>
       </c>
       <c r="C3">
         <v>0.6</v>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
-        <v>-245753.44032150001</v>
+        <v>-347904.04412999999</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="1"/>
@@ -4100,7 +4100,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>163835.626881</v>
+        <v>231936.02942000001</v>
       </c>
       <c r="D4">
         <f t="shared" si="3"/>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>-163835.626881</v>
+        <v>-231936.02942000001</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>-81917.813440500002</v>
+        <v>-115968.01471</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
@@ -4174,15 +4174,15 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>81917.813440500002</v>
+        <v>115968.01471</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>6.3972830989308099E-3</v>
+        <v>9.9873995490428573E-3</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="2"/>
-        <v>1.1157556955946986E-2</v>
+        <v>1.5984873107996855E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
       </c>
       <c r="B8" s="4">
         <f>ABS(I36)+ABS(I37)</f>
-        <v>1.0207138994302832E-3</v>
+        <v>5.3406108603053226E-4</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
@@ -4199,15 +4199,15 @@
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>163835.626881</v>
+        <v>231936.02942000001</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>1.018763801755296E-2</v>
+        <v>1.4272852052126977E-2</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="2"/>
-        <v>1.6223757300038305E-2</v>
+        <v>2.039713187617774E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4223,15 +4223,15 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>245753.44032150001</v>
+        <v>347904.04412999999</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>1.2694846923443645E-2</v>
+        <v>1.6654993044984981E-2</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="2"/>
-        <v>1.8943328310500624E-2</v>
+        <v>2.2214434356830043E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4241,15 +4241,15 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>327671.25376200001</v>
+        <v>463872.05884000001</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>1.4476160651179501E-2</v>
+        <v>1.8171397423826743E-2</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="2"/>
-        <v>2.0569952214408695E-2</v>
+        <v>2.3134807474267202E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4259,15 +4259,15 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>409589.06720250001</v>
+        <v>579840.07354999997</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>1.5806959904178033E-2</v>
+        <v>1.9221442138250947E-2</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="2"/>
-        <v>2.1619520551864387E-2</v>
+        <v>2.3664330761536727E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4278,15 +4278,15 @@
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>491506.88064300001</v>
+        <v>695808.08825999999</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>1.683896866490299E-2</v>
+        <v>1.9991592636924165E-2</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="2"/>
-        <v>2.2335902701902593E-2</v>
+        <v>2.3996634227419517E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4297,15 +4297,15 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>573424.69408349996</v>
+        <v>811776.10297000001</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>1.7662657231337399E-2</v>
+        <v>2.058059847073759E-2</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="2"/>
-        <v>2.2846536043806185E-2</v>
+        <v>2.4218755604926128E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4315,15 +4315,15 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>655342.50752400002</v>
+        <v>927744.11768000002</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>1.8335319864429333E-2</v>
+        <v>2.1045644232259391E-2</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="2"/>
-        <v>2.3223281547621193E-2</v>
+        <v>2.4374522818485466E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4333,15 +4333,15 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>737260.32096450008</v>
+        <v>1043712.13239</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>1.889500504113676E-2</v>
+        <v>2.1422136449261449E-2</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="2"/>
-        <v>2.3509161462090186E-2</v>
+        <v>2.4487955696491863E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4351,15 +4351,15 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>819178.13440500002</v>
+        <v>1159680.1470999999</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>1.9367970489955113E-2</v>
+        <v>2.1733169712283833E-2</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="2"/>
-        <v>2.3731209743919346E-2</v>
+        <v>2.4573112794850409E-2</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
@@ -4369,15 +4369,15 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>901095.94784549996</v>
+        <v>1275648.16181</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>1.9772922055468628E-2</v>
+        <v>2.1994450207187485E-2</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="2"/>
-        <v>2.3907106246471747E-2</v>
+        <v>2.4638666817716984E-2</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
@@ -4387,15 +4387,15 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>983013.76128600002</v>
+        <v>1391616.17652</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>2.0123546543139956E-2</v>
+        <v>2.2217031522148493E-2</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="2"/>
-        <v>2.404880806732311E-2</v>
+        <v>2.4690203458051403E-2</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
@@ -4405,15 +4405,15 @@
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>1064931.5747265001</v>
+        <v>1507584.19123</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>2.0430089248805482E-2</v>
+        <v>2.2408918642781106E-2</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="2"/>
-        <v>2.416463662904467E-2</v>
+        <v>2.4731451896010916E-2</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
@@ -4423,15 +4423,15 @@
       </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>1146849.3881669999</v>
+        <v>1623552.20594</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>2.0700371680509724E-2</v>
+        <v>2.2576051172244024E-2</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="2"/>
-        <v>2.4260527852569488E-2</v>
+        <v>2.4764978883216826E-2</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
@@ -4441,15 +4441,15 @@
       </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>1228767.2016075</v>
+        <v>1739520.22065</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>2.0940468295190761E-2</v>
+        <v>2.2722929085094684E-2</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="2"/>
-        <v>2.4340808093505938E-2</v>
+        <v>2.4792597921939694E-2</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
@@ -4459,15 +4459,15 @@
       </c>
       <c r="E22" s="2">
         <f t="shared" si="0"/>
-        <v>1310685.015048</v>
+        <v>1855488.23536</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>2.1155168488186701E-2</v>
+        <v>2.2853023975626014E-2</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="2"/>
-        <v>2.4408690825830699E-2</v>
+        <v>2.4815619758030535E-2</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
@@ -4477,15 +4477,15 @@
       </c>
       <c r="E23" s="2">
         <f t="shared" si="0"/>
-        <v>1392602.8284885001</v>
+        <v>1971456.2500700001</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>2.1348299344761672E-2</v>
+        <v>2.2969056951100117E-2</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="2"/>
-        <v>2.4466603292981282E-2</v>
+        <v>2.483501081328501E-2</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
@@ -4495,15 +4495,15 @@
       </c>
       <c r="E24" s="2">
         <f t="shared" si="0"/>
-        <v>1474520.6419290002</v>
+        <v>2087424.2647800001</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>2.1522955770740961E-2</v>
+        <v>2.3073191033199707E-2</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="2"/>
-        <v>2.4516406537111061E-2</v>
+        <v>2.4851496288218318E-2</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
@@ -4513,15 +4513,15 @@
       </c>
       <c r="E25" s="2">
         <f t="shared" si="0"/>
-        <v>1556438.4553695</v>
+        <v>2203392.2794900001</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>2.168166759641852E-2</v>
+        <v>2.3167167255522449E-2</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="2"/>
-        <v>2.4559546802373645E-2</v>
+        <v>2.4865628965230833E-2</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
@@ -4531,15 +4531,15 @@
       </c>
       <c r="E26" s="2">
         <f t="shared" si="0"/>
-        <v>1638356.26881</v>
+        <v>2319360.2941999999</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>2.182652291289728E-2</v>
+        <v>2.3252402785950189E-2</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="2"/>
-        <v>2.4597161727105361E-2</v>
+        <v>2.4877836159097812E-2</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
@@ -4549,15 +4549,15 @@
       </c>
       <c r="E27" s="2">
         <f t="shared" si="0"/>
-        <v>1720274.0822505001</v>
+        <v>2435328.3089100001</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>2.1959260455574395E-2</v>
+        <v>2.333006288672055E-2</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="2"/>
-        <v>2.4630156120918657E-2</v>
+        <v>2.4888452401507683E-2</v>
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
@@ -4567,15 +4567,15 @@
       </c>
       <c r="E28" s="2">
         <f t="shared" si="0"/>
-        <v>1802191.8956909999</v>
+        <v>2551296.3236199999</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>2.2081339733614209E-2</v>
+        <v>2.3401114504179883E-2</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="2"/>
-        <v>2.4659256889976829E-2</v>
+        <v>2.4897742606850248E-2</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
@@ -4585,15 +4585,15 @@
       </c>
       <c r="E29" s="2">
         <f t="shared" si="0"/>
-        <v>1884109.7091315</v>
+        <v>2667264.3383300002</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>2.2193994918170791E-2</v>
+        <v>2.3466366736204426E-2</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="2"/>
-        <v>2.4685053419229951E-2</v>
+        <v>2.4905918760487197E-2</v>
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
@@ -4603,15 +4603,15 @@
       </c>
       <c r="E30" s="2">
         <f t="shared" si="0"/>
-        <v>1966027.522572</v>
+        <v>2783232.35304</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
-        <v>2.2298276714465499E-2</v>
+        <v>2.3526501779052925E-2</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="2"/>
-        <v>2.4708027651536024E-2</v>
+        <v>2.4913152119714635E-2</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
@@ -4621,15 +4621,15 @@
       </c>
       <c r="E31" s="2">
         <f t="shared" si="0"/>
-        <v>2047945.3360125001</v>
+        <v>2899200.3677500002</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
-        <v>2.2395085231668582E-2</v>
+        <v>2.3582098868218555E-2</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="2"/>
-        <v>2.4728576761989158E-2</v>
+        <v>2.4919582255219713E-2</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
@@ -4639,15 +4639,15 @@
       </c>
       <c r="E32" s="2">
         <f t="shared" si="0"/>
-        <v>2129863.1494530002</v>
+        <v>3015168.38246</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
-        <v>2.2485196030450967E-2</v>
+        <v>2.3633652996421256E-2</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="2"/>
-        <v>2.4747030439789621E-2</v>
+        <v>2.4925323834632456E-2</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -4657,15 +4657,15 @@
       </c>
       <c r="E33" s="2">
         <f t="shared" si="0"/>
-        <v>2211780.9628935</v>
+        <v>3131136.3971700002</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
-        <v>2.2569280944984765E-2</v>
+        <v>2.3681589691406196E-2</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="2"/>
-        <v>2.4763664195023436E-2</v>
+        <v>2.4930471770327742E-2</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -4675,15 +4675,15 @@
       </c>
       <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>2293698.7763339998</v>
+        <v>3247104.41188</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
-        <v>2.2647924862871531E-2</v>
+        <v>2.3726276788409606E-2</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="2"/>
-        <v>2.4778709701972084E-2</v>
+        <v>2.4935105167210238E-2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -4692,15 +4692,15 @@
       </c>
       <c r="E35" s="2">
         <f t="shared" ref="E35" si="4">f*D35</f>
-        <v>1638356.26881</v>
+        <v>2319360.2941999999</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
-        <v>2.182652291289728E-2</v>
+        <v>2.3252402785950189E-2</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" ref="G35" si="5">IF(D35-bmin&gt;0,p*(2*h*m*(D35-bmin)+h^2*(D35-bmin)^2)/(h*(D35-bmin)+m)^2,0)</f>
-        <v>2.4597161727105361E-2</v>
+        <v>2.4877836159097812E-2</v>
       </c>
       <c r="H35" t="s">
         <v>12</v>
@@ -4712,52 +4712,52 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>E36/f</f>
-        <v>0.96930298000000004</v>
+        <v>0.50105135999999995</v>
       </c>
       <c r="E36" s="5">
         <f>B42</f>
-        <v>158806.36136592142</v>
+        <v>116211.86297389099</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
-        <v>9.9999999400160588E-3</v>
+        <v>9.9999999719342907E-3</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" ref="G36:G37" si="6">IF(D36-bmin&gt;0,p*(2*h*m*(D36-bmin)+h^2*(D36-bmin)^2)/(h*(D36-bmin)+m)^2,0)</f>
-        <v>1.599999992801927E-2</v>
+        <v>1.5999999966321152E-2</v>
       </c>
       <c r="H36" s="9">
         <v>0.01</v>
       </c>
       <c r="I36" s="8">
         <f>F36-H36</f>
-        <v>-5.9983941425034715E-11</v>
+        <v>-2.8065709478664047E-11</v>
       </c>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" s="4">
         <f>E37/f</f>
-        <v>7.6805637799999991</v>
+        <v>3.4556963500000002</v>
       </c>
       <c r="E37" s="5">
         <f>H42</f>
-        <v>1258349.9816958029</v>
+        <v>801500.49030018668</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="1"/>
-        <v>2.1020713839446342E-2</v>
+        <v>2.0534061057964823E-2</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="6"/>
-        <v>2.4366611266097047E-2</v>
+        <v>2.4202215574640553E-2</v>
       </c>
       <c r="H37" s="9">
         <v>0.02</v>
       </c>
       <c r="I37" s="8">
         <f>F37-H37</f>
-        <v>1.0207138394463418E-3</v>
+        <v>5.3406105796482278E-4</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -4796,92 +4796,92 @@
         <v>10</v>
       </c>
       <c r="B41" s="4">
-        <v>0.96930298000000004</v>
+        <v>0.50105135999999995</v>
       </c>
       <c r="C41" s="4">
-        <v>1.2167460400000001</v>
+        <v>0.65197760999999999</v>
       </c>
       <c r="D41" s="4">
-        <v>1.42650539</v>
+        <v>0.75971648000000003</v>
       </c>
       <c r="E41" s="4">
-        <v>1.6231236499999999</v>
+        <v>0.84668591000000004</v>
       </c>
       <c r="F41" s="7">
-        <v>1.88237802</v>
+        <v>0.95077845000000005</v>
       </c>
       <c r="G41" s="7">
-        <v>2.6704851600000001</v>
+        <v>1.2536148899999999</v>
       </c>
       <c r="H41" s="4">
-        <v>7.68056378</v>
+        <v>3.4556963500000002</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>163835.626881</v>
+        <v>231936.02942000001</v>
       </c>
       <c r="B42" s="6">
         <f t="shared" ref="B42:H42" si="7">B41*sim_conv</f>
-        <v>158806.36136592142</v>
+        <v>116211.86297389099</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="7"/>
-        <v>199346.35021837431</v>
+        <v>151217.0981341413</v>
       </c>
       <c r="D42" s="6">
         <f t="shared" si="7"/>
-        <v>233712.4048197754</v>
+        <v>176205.62385613885</v>
       </c>
       <c r="E42" s="6">
         <f t="shared" si="7"/>
-        <v>265925.48070312681</v>
+        <v>196376.96813125949</v>
       </c>
       <c r="F42" s="6">
         <f t="shared" si="7"/>
-        <v>308400.58293371554</v>
+        <v>220519.778551102</v>
       </c>
       <c r="G42" s="6">
         <f t="shared" si="7"/>
-        <v>437520.61026500759</v>
+        <v>290758.46000839007</v>
       </c>
       <c r="H42" s="6">
         <f t="shared" si="7"/>
-        <v>1258349.9816958029</v>
+        <v>801500.49030018668</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5">
         <f>B40*B42</f>
-        <v>39701.590341480354</v>
+        <v>29052.965743472749</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" ref="C43:H43" si="8">C40*C42</f>
-        <v>49836.587554593578</v>
+        <v>37804.274533535325</v>
       </c>
       <c r="D43" s="5">
         <f t="shared" si="8"/>
-        <v>46742.48096395508</v>
+        <v>35241.124771227769</v>
       </c>
       <c r="E43" s="5">
         <f t="shared" si="8"/>
-        <v>26592.548070312681</v>
+        <v>19637.696813125949</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="8"/>
-        <v>30840.058293371556</v>
+        <v>22051.977855110203</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="8"/>
-        <v>39376.854923850682</v>
+        <v>26168.261400755106</v>
       </c>
       <c r="H43" s="5">
         <f t="shared" si="8"/>
-        <v>12583.499816958029</v>
+        <v>8015.0049030018672</v>
       </c>
       <c r="I43" s="5">
         <f>SUM(B43:H43)</f>
-        <v>245673.61996452196</v>
+        <v>177971.30602022895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
baseline simulation finished, calibrated wealth tax parameters, fixed an SS.py error
</commit_message>
<xml_diff>
--- a/Data/Effective Wealth Tax Rates.xlsx
+++ b/Data/Effective Wealth Tax Rates.xlsx
@@ -360,103 +360,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-463872.05884000001</c:v>
+                  <c:v>-420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-347904.04412999999</c:v>
+                  <c:v>-315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-231936.02942000001</c:v>
+                  <c:v>-210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-115968.01471</c:v>
+                  <c:v>-105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>115968.01471</c:v>
+                  <c:v>105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>231936.02942000001</c:v>
+                  <c:v>210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>347904.04412999999</c:v>
+                  <c:v>315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>463872.05884000001</c:v>
+                  <c:v>420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>579840.07354999997</c:v>
+                  <c:v>526041.39121250005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>695808.08825999999</c:v>
+                  <c:v>631249.66945499997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>811776.10297000001</c:v>
+                  <c:v>736457.9476975</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>927744.11768000002</c:v>
+                  <c:v>841666.22594000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1043712.13239</c:v>
+                  <c:v>946874.50418250007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1159680.1470999999</c:v>
+                  <c:v>1052082.7824250001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1275648.16181</c:v>
+                  <c:v>1157291.0606675001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1391616.17652</c:v>
+                  <c:v>1262499.3389099999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1507584.19123</c:v>
+                  <c:v>1367707.6171525</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1623552.20594</c:v>
+                  <c:v>1472915.895395</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1739520.22065</c:v>
+                  <c:v>1578124.1736375</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1855488.23536</c:v>
+                  <c:v>1683332.4518800001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1971456.2500700001</c:v>
+                  <c:v>1788540.7301225001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2087424.2647800001</c:v>
+                  <c:v>1893749.0083650001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2203392.2794900001</c:v>
+                  <c:v>1998957.2866075002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2319360.2941999999</c:v>
+                  <c:v>2104165.5648500002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2435328.3089100001</c:v>
+                  <c:v>2209373.8430925002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2551296.3236199999</c:v>
+                  <c:v>2314582.1213350003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2667264.3383300002</c:v>
+                  <c:v>2419790.3995775003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2783232.35304</c:v>
+                  <c:v>2524998.6778199999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2899200.3677500002</c:v>
+                  <c:v>2630206.9560624999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3015168.38246</c:v>
+                  <c:v>2735415.2343049999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3131136.3971700002</c:v>
+                  <c:v>2840623.5125475</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3247104.41188</c:v>
+                  <c:v>2945831.79079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -483,88 +483,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9873995490428573E-3</c:v>
+                  <c:v>8.6158149537096575E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4272852052126977E-2</c:v>
+                  <c:v>1.2815121343293304E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6654993044984981E-2</c:v>
+                  <c:v>1.5300998870865303E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8171397423826743E-2</c:v>
+                  <c:v>1.6944440329775812E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9221442138250947E-2</c:v>
+                  <c:v>1.8111635194022029E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.9991592636924165E-2</c:v>
+                  <c:v>1.8983399046626132E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.058059847073759E-2</c:v>
+                  <c:v>1.9659297019128701E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.1045644232259391E-2</c:v>
+                  <c:v>2.0198672573236334E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1422136449261449E-2</c:v>
+                  <c:v>2.0639095031177557E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1733169712283833E-2</c:v>
+                  <c:v>2.1005507112536334E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1994450207187485E-2</c:v>
+                  <c:v>2.131511834388209E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2217031522148493E-2</c:v>
+                  <c:v>2.1580186454555408E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2408918642781106E-2</c:v>
+                  <c:v>2.1809678870627933E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2576051172244024E-2</c:v>
+                  <c:v>2.2010307294702967E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2722929085094684E-2</c:v>
+                  <c:v>2.2187195014935383E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2853023975626014E-2</c:v>
+                  <c:v>2.2344320555551727E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.2969056951100117E-2</c:v>
+                  <c:v>2.248482049816132E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3073191033199707E-2</c:v>
+                  <c:v>2.2611201007686849E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3167167255522449E-2</c:v>
+                  <c:v>2.2725488637914373E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3252402785950189E-2</c:v>
+                  <c:v>2.2829339823549524E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.333006288672055E-2</c:v>
+                  <c:v>2.292412168645408E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3401114504179883E-2</c:v>
+                  <c:v>2.3010972557190573E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3466366736204426E-2</c:v>
+                  <c:v>2.309084791402315E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3526501779052925E-2</c:v>
+                  <c:v>2.3164555680352937E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3582098868218555E-2</c:v>
+                  <c:v>2.3232783649599732E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3633652996421256E-2</c:v>
+                  <c:v>2.3296121012606478E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3681589691406196E-2</c:v>
+                  <c:v>2.3355075415940126E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3726276788409606E-2</c:v>
+                  <c:v>2.3410086597309959E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,11 +579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="243999144"/>
-        <c:axId val="243999536"/>
+        <c:axId val="238146728"/>
+        <c:axId val="238147512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="243999144"/>
+        <c:axId val="238146728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,12 +640,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243999536"/>
+        <c:crossAx val="238147512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="243999536"/>
+        <c:axId val="238147512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243999144"/>
+        <c:crossAx val="238146728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -861,103 +861,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-463872.05884000001</c:v>
+                  <c:v>-420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-347904.04412999999</c:v>
+                  <c:v>-315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-231936.02942000001</c:v>
+                  <c:v>-210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-115968.01471</c:v>
+                  <c:v>-105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>115968.01471</c:v>
+                  <c:v>105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>231936.02942000001</c:v>
+                  <c:v>210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>347904.04412999999</c:v>
+                  <c:v>315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>463872.05884000001</c:v>
+                  <c:v>420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>579840.07354999997</c:v>
+                  <c:v>526041.39121250005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>695808.08825999999</c:v>
+                  <c:v>631249.66945499997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>811776.10297000001</c:v>
+                  <c:v>736457.9476975</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>927744.11768000002</c:v>
+                  <c:v>841666.22594000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1043712.13239</c:v>
+                  <c:v>946874.50418250007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1159680.1470999999</c:v>
+                  <c:v>1052082.7824250001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1275648.16181</c:v>
+                  <c:v>1157291.0606675001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1391616.17652</c:v>
+                  <c:v>1262499.3389099999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1507584.19123</c:v>
+                  <c:v>1367707.6171525</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1623552.20594</c:v>
+                  <c:v>1472915.895395</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1739520.22065</c:v>
+                  <c:v>1578124.1736375</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1855488.23536</c:v>
+                  <c:v>1683332.4518800001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1971456.2500700001</c:v>
+                  <c:v>1788540.7301225001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2087424.2647800001</c:v>
+                  <c:v>1893749.0083650001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2203392.2794900001</c:v>
+                  <c:v>1998957.2866075002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2319360.2941999999</c:v>
+                  <c:v>2104165.5648500002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2435328.3089100001</c:v>
+                  <c:v>2209373.8430925002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2551296.3236199999</c:v>
+                  <c:v>2314582.1213350003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2667264.3383300002</c:v>
+                  <c:v>2419790.3995775003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2783232.35304</c:v>
+                  <c:v>2524998.6778199999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2899200.3677500002</c:v>
+                  <c:v>2630206.9560624999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3015168.38246</c:v>
+                  <c:v>2735415.2343049999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3131136.3971700002</c:v>
+                  <c:v>2840623.5125475</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3247104.41188</c:v>
+                  <c:v>2945831.79079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,88 +984,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5984873107996855E-2</c:v>
+                  <c:v>1.4262339214756638E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.039713187617774E-2</c:v>
+                  <c:v>1.9061149284853345E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2214434356830043E-2</c:v>
+                  <c:v>2.1237175083881756E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3134807474267202E-2</c:v>
+                  <c:v>2.2404318335978304E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3664330761536727E-2</c:v>
+                  <c:v>2.3102017211990566E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3996634227419517E-2</c:v>
+                  <c:v>2.3552020518714432E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.4218755604926128E-2</c:v>
+                  <c:v>2.3859075666804497E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4374522818485466E-2</c:v>
+                  <c:v>2.4077890197640284E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4487955696491863E-2</c:v>
+                  <c:v>2.4239300314115992E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4573112794850409E-2</c:v>
+                  <c:v>2.4361761062880089E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4638666817716984E-2</c:v>
+                  <c:v>2.4456865887216236E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4690203458051403E-2</c:v>
+                  <c:v>2.4532195012575753E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.4731451896010916E-2</c:v>
+                  <c:v>2.4592874043659282E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4764978883216826E-2</c:v>
+                  <c:v>2.4642469501115743E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4792597921939694E-2</c:v>
+                  <c:v>2.4683525124639828E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4815619758030535E-2</c:v>
+                  <c:v>2.4717894667533394E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.483501081328501E-2</c:v>
+                  <c:v>2.4746954882941218E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4851496288218318E-2</c:v>
+                  <c:v>2.4771745574972949E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.4865628965230833E-2</c:v>
+                  <c:v>2.4793063922549739E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4877836159097812E-2</c:v>
+                  <c:v>2.4811529375934876E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4888452401507683E-2</c:v>
+                  <c:v>2.4827629169093993E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4897742606850248E-2</c:v>
+                  <c:v>2.4841750793270036E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4905918760487197E-2</c:v>
+                  <c:v>2.4854205532504413E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4913152119714635E-2</c:v>
+                  <c:v>2.4865245765979017E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4919582255219713E-2</c:v>
+                  <c:v>2.4875077854835118E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4925323834632456E-2</c:v>
+                  <c:v>2.4883871855852759E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.4930471770327742E-2</c:v>
+                  <c:v>2.489176892451022E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4935105167210238E-2</c:v>
+                  <c:v>2.4898887014877857E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,11 +1080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="244000320"/>
-        <c:axId val="244000712"/>
+        <c:axId val="238148296"/>
+        <c:axId val="196573888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="244000320"/>
+        <c:axId val="238148296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,12 +1141,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244000712"/>
+        <c:crossAx val="196573888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="244000712"/>
+        <c:axId val="196573888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244000320"/>
+        <c:crossAx val="238148296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1300,103 +1300,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-463872.05884000001</c:v>
+                  <c:v>-420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-347904.04412999999</c:v>
+                  <c:v>-315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-231936.02942000001</c:v>
+                  <c:v>-210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-115968.01471</c:v>
+                  <c:v>-105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>115968.01471</c:v>
+                  <c:v>105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>231936.02942000001</c:v>
+                  <c:v>210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>347904.04412999999</c:v>
+                  <c:v>315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>463872.05884000001</c:v>
+                  <c:v>420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>579840.07354999997</c:v>
+                  <c:v>526041.39121250005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>695808.08825999999</c:v>
+                  <c:v>631249.66945499997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>811776.10297000001</c:v>
+                  <c:v>736457.9476975</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>927744.11768000002</c:v>
+                  <c:v>841666.22594000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1043712.13239</c:v>
+                  <c:v>946874.50418250007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1159680.1470999999</c:v>
+                  <c:v>1052082.7824250001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1275648.16181</c:v>
+                  <c:v>1157291.0606675001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1391616.17652</c:v>
+                  <c:v>1262499.3389099999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1507584.19123</c:v>
+                  <c:v>1367707.6171525</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1623552.20594</c:v>
+                  <c:v>1472915.895395</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1739520.22065</c:v>
+                  <c:v>1578124.1736375</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1855488.23536</c:v>
+                  <c:v>1683332.4518800001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1971456.2500700001</c:v>
+                  <c:v>1788540.7301225001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2087424.2647800001</c:v>
+                  <c:v>1893749.0083650001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2203392.2794900001</c:v>
+                  <c:v>1998957.2866075002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2319360.2941999999</c:v>
+                  <c:v>2104165.5648500002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2435328.3089100001</c:v>
+                  <c:v>2209373.8430925002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2551296.3236199999</c:v>
+                  <c:v>2314582.1213350003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2667264.3383300002</c:v>
+                  <c:v>2419790.3995775003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2783232.35304</c:v>
+                  <c:v>2524998.6778199999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2899200.3677500002</c:v>
+                  <c:v>2630206.9560624999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3015168.38246</c:v>
+                  <c:v>2735415.2343049999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3131136.3971700002</c:v>
+                  <c:v>2840623.5125475</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3247104.41188</c:v>
+                  <c:v>2945831.79079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1423,88 +1423,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9873995490428573E-3</c:v>
+                  <c:v>8.6158149537096575E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4272852052126977E-2</c:v>
+                  <c:v>1.2815121343293304E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6654993044984981E-2</c:v>
+                  <c:v>1.5300998870865303E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8171397423826743E-2</c:v>
+                  <c:v>1.6944440329775812E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9221442138250947E-2</c:v>
+                  <c:v>1.8111635194022029E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.9991592636924165E-2</c:v>
+                  <c:v>1.8983399046626132E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.058059847073759E-2</c:v>
+                  <c:v>1.9659297019128701E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.1045644232259391E-2</c:v>
+                  <c:v>2.0198672573236334E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1422136449261449E-2</c:v>
+                  <c:v>2.0639095031177557E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1733169712283833E-2</c:v>
+                  <c:v>2.1005507112536334E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1994450207187485E-2</c:v>
+                  <c:v>2.131511834388209E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2217031522148493E-2</c:v>
+                  <c:v>2.1580186454555408E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2408918642781106E-2</c:v>
+                  <c:v>2.1809678870627933E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2576051172244024E-2</c:v>
+                  <c:v>2.2010307294702967E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2722929085094684E-2</c:v>
+                  <c:v>2.2187195014935383E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2853023975626014E-2</c:v>
+                  <c:v>2.2344320555551727E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.2969056951100117E-2</c:v>
+                  <c:v>2.248482049816132E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3073191033199707E-2</c:v>
+                  <c:v>2.2611201007686849E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3167167255522449E-2</c:v>
+                  <c:v>2.2725488637914373E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3252402785950189E-2</c:v>
+                  <c:v>2.2829339823549524E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.333006288672055E-2</c:v>
+                  <c:v>2.292412168645408E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3401114504179883E-2</c:v>
+                  <c:v>2.3010972557190573E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3466366736204426E-2</c:v>
+                  <c:v>2.309084791402315E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3526501779052925E-2</c:v>
+                  <c:v>2.3164555680352937E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3582098868218555E-2</c:v>
+                  <c:v>2.3232783649599732E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3633652996421256E-2</c:v>
+                  <c:v>2.3296121012606478E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3681589691406196E-2</c:v>
+                  <c:v>2.3355075415940126E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3726276788409606E-2</c:v>
+                  <c:v>2.3410086597309959E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1547,103 +1547,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-463872.05884000001</c:v>
+                  <c:v>-420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-347904.04412999999</c:v>
+                  <c:v>-315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-231936.02942000001</c:v>
+                  <c:v>-210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-115968.01471</c:v>
+                  <c:v>-105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>115968.01471</c:v>
+                  <c:v>105208.2782425</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>231936.02942000001</c:v>
+                  <c:v>210416.55648500001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>347904.04412999999</c:v>
+                  <c:v>315624.83472749998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>463872.05884000001</c:v>
+                  <c:v>420833.11297000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>579840.07354999997</c:v>
+                  <c:v>526041.39121250005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>695808.08825999999</c:v>
+                  <c:v>631249.66945499997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>811776.10297000001</c:v>
+                  <c:v>736457.9476975</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>927744.11768000002</c:v>
+                  <c:v>841666.22594000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1043712.13239</c:v>
+                  <c:v>946874.50418250007</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1159680.1470999999</c:v>
+                  <c:v>1052082.7824250001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1275648.16181</c:v>
+                  <c:v>1157291.0606675001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1391616.17652</c:v>
+                  <c:v>1262499.3389099999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1507584.19123</c:v>
+                  <c:v>1367707.6171525</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1623552.20594</c:v>
+                  <c:v>1472915.895395</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1739520.22065</c:v>
+                  <c:v>1578124.1736375</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1855488.23536</c:v>
+                  <c:v>1683332.4518800001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1971456.2500700001</c:v>
+                  <c:v>1788540.7301225001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2087424.2647800001</c:v>
+                  <c:v>1893749.0083650001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2203392.2794900001</c:v>
+                  <c:v>1998957.2866075002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2319360.2941999999</c:v>
+                  <c:v>2104165.5648500002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2435328.3089100001</c:v>
+                  <c:v>2209373.8430925002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2551296.3236199999</c:v>
+                  <c:v>2314582.1213350003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2667264.3383300002</c:v>
+                  <c:v>2419790.3995775003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2783232.35304</c:v>
+                  <c:v>2524998.6778199999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2899200.3677500002</c:v>
+                  <c:v>2630206.9560624999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3015168.38246</c:v>
+                  <c:v>2735415.2343049999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3131136.3971700002</c:v>
+                  <c:v>2840623.5125475</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3247104.41188</c:v>
+                  <c:v>2945831.79079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,88 +1670,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5984873107996855E-2</c:v>
+                  <c:v>1.4262339214756638E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.039713187617774E-2</c:v>
+                  <c:v>1.9061149284853345E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2214434356830043E-2</c:v>
+                  <c:v>2.1237175083881756E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3134807474267202E-2</c:v>
+                  <c:v>2.2404318335978304E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3664330761536727E-2</c:v>
+                  <c:v>2.3102017211990566E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3996634227419517E-2</c:v>
+                  <c:v>2.3552020518714432E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.4218755604926128E-2</c:v>
+                  <c:v>2.3859075666804497E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4374522818485466E-2</c:v>
+                  <c:v>2.4077890197640284E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4487955696491863E-2</c:v>
+                  <c:v>2.4239300314115992E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4573112794850409E-2</c:v>
+                  <c:v>2.4361761062880089E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4638666817716984E-2</c:v>
+                  <c:v>2.4456865887216236E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4690203458051403E-2</c:v>
+                  <c:v>2.4532195012575753E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.4731451896010916E-2</c:v>
+                  <c:v>2.4592874043659282E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4764978883216826E-2</c:v>
+                  <c:v>2.4642469501115743E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4792597921939694E-2</c:v>
+                  <c:v>2.4683525124639828E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4815619758030535E-2</c:v>
+                  <c:v>2.4717894667533394E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.483501081328501E-2</c:v>
+                  <c:v>2.4746954882941218E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4851496288218318E-2</c:v>
+                  <c:v>2.4771745574972949E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.4865628965230833E-2</c:v>
+                  <c:v>2.4793063922549739E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4877836159097812E-2</c:v>
+                  <c:v>2.4811529375934876E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4888452401507683E-2</c:v>
+                  <c:v>2.4827629169093993E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4897742606850248E-2</c:v>
+                  <c:v>2.4841750793270036E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4905918760487197E-2</c:v>
+                  <c:v>2.4854205532504413E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4913152119714635E-2</c:v>
+                  <c:v>2.4865245765979017E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4919582255219713E-2</c:v>
+                  <c:v>2.4875077854835118E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4925323834632456E-2</c:v>
+                  <c:v>2.4883871855852759E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.4930471770327742E-2</c:v>
+                  <c:v>2.489176892451022E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4935105167210238E-2</c:v>
+                  <c:v>2.4898887014877857E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1766,11 +1766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="244919936"/>
-        <c:axId val="244920328"/>
+        <c:axId val="196574672"/>
+        <c:axId val="196575064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="244919936"/>
+        <c:axId val="196574672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,12 +1827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244920328"/>
+        <c:crossAx val="196575064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="244920328"/>
+        <c:axId val="196575064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,7 +1889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244919936"/>
+        <c:crossAx val="196574672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.01"/>
@@ -4017,7 +4017,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4047,7 +4047,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.36350750271454</v>
+        <v>1.1867121650630199</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E34" si="0">f*D2</f>
-        <v>-463872.05884000001</v>
+        <v>-420833.11297000002</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F37" si="1">IF(D2-bmin&gt;0,p*(h*D2-bmin)/(h*D2-bmin+m),0)</f>
@@ -4073,7 +4073,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.02478093770152</v>
+        <v>1.12835012204532</v>
       </c>
       <c r="C3">
         <v>0.6</v>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
-        <v>-347904.04412999999</v>
+        <v>-315624.83472749998</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="1"/>
@@ -4100,7 +4100,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>231936.02942000001</v>
+        <v>210416.55648500001</v>
       </c>
       <c r="D4">
         <f t="shared" si="3"/>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>-231936.02942000001</v>
+        <v>-210416.55648500001</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>-115968.01471</v>
+        <v>-105208.2782425</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
@@ -4174,15 +4174,15 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>115968.01471</v>
+        <v>105208.2782425</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>9.9873995490428573E-3</v>
+        <v>8.6158149537096575E-3</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="2"/>
-        <v>1.5984873107996855E-2</v>
+        <v>1.4262339214756638E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
       </c>
       <c r="B8" s="4">
         <f>ABS(I36)+ABS(I37)</f>
-        <v>5.3406108603053226E-4</v>
+        <v>1.5696268409532387E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
@@ -4199,15 +4199,15 @@
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>231936.02942000001</v>
+        <v>210416.55648500001</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>1.4272852052126977E-2</v>
+        <v>1.2815121343293304E-2</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="2"/>
-        <v>2.039713187617774E-2</v>
+        <v>1.9061149284853345E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4223,15 +4223,15 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>347904.04412999999</v>
+        <v>315624.83472749998</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>1.6654993044984981E-2</v>
+        <v>1.5300998870865303E-2</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="2"/>
-        <v>2.2214434356830043E-2</v>
+        <v>2.1237175083881756E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4241,15 +4241,15 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>463872.05884000001</v>
+        <v>420833.11297000002</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>1.8171397423826743E-2</v>
+        <v>1.6944440329775812E-2</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="2"/>
-        <v>2.3134807474267202E-2</v>
+        <v>2.2404318335978304E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4259,15 +4259,15 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>579840.07354999997</v>
+        <v>526041.39121250005</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>1.9221442138250947E-2</v>
+        <v>1.8111635194022029E-2</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="2"/>
-        <v>2.3664330761536727E-2</v>
+        <v>2.3102017211990566E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4278,15 +4278,15 @@
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>695808.08825999999</v>
+        <v>631249.66945499997</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>1.9991592636924165E-2</v>
+        <v>1.8983399046626132E-2</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="2"/>
-        <v>2.3996634227419517E-2</v>
+        <v>2.3552020518714432E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4297,15 +4297,15 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>811776.10297000001</v>
+        <v>736457.9476975</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>2.058059847073759E-2</v>
+        <v>1.9659297019128701E-2</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="2"/>
-        <v>2.4218755604926128E-2</v>
+        <v>2.3859075666804497E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4315,15 +4315,15 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>927744.11768000002</v>
+        <v>841666.22594000003</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>2.1045644232259391E-2</v>
+        <v>2.0198672573236334E-2</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="2"/>
-        <v>2.4374522818485466E-2</v>
+        <v>2.4077890197640284E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4333,15 +4333,15 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>1043712.13239</v>
+        <v>946874.50418250007</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>2.1422136449261449E-2</v>
+        <v>2.0639095031177557E-2</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="2"/>
-        <v>2.4487955696491863E-2</v>
+        <v>2.4239300314115992E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4351,15 +4351,15 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>1159680.1470999999</v>
+        <v>1052082.7824250001</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>2.1733169712283833E-2</v>
+        <v>2.1005507112536334E-2</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="2"/>
-        <v>2.4573112794850409E-2</v>
+        <v>2.4361761062880089E-2</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
@@ -4369,15 +4369,15 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>1275648.16181</v>
+        <v>1157291.0606675001</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>2.1994450207187485E-2</v>
+        <v>2.131511834388209E-2</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="2"/>
-        <v>2.4638666817716984E-2</v>
+        <v>2.4456865887216236E-2</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
@@ -4387,15 +4387,15 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>1391616.17652</v>
+        <v>1262499.3389099999</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>2.2217031522148493E-2</v>
+        <v>2.1580186454555408E-2</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="2"/>
-        <v>2.4690203458051403E-2</v>
+        <v>2.4532195012575753E-2</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
@@ -4405,15 +4405,15 @@
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>1507584.19123</v>
+        <v>1367707.6171525</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>2.2408918642781106E-2</v>
+        <v>2.1809678870627933E-2</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="2"/>
-        <v>2.4731451896010916E-2</v>
+        <v>2.4592874043659282E-2</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
@@ -4423,15 +4423,15 @@
       </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>1623552.20594</v>
+        <v>1472915.895395</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>2.2576051172244024E-2</v>
+        <v>2.2010307294702967E-2</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="2"/>
-        <v>2.4764978883216826E-2</v>
+        <v>2.4642469501115743E-2</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
@@ -4441,15 +4441,15 @@
       </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>1739520.22065</v>
+        <v>1578124.1736375</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>2.2722929085094684E-2</v>
+        <v>2.2187195014935383E-2</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="2"/>
-        <v>2.4792597921939694E-2</v>
+        <v>2.4683525124639828E-2</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
@@ -4459,15 +4459,15 @@
       </c>
       <c r="E22" s="2">
         <f t="shared" si="0"/>
-        <v>1855488.23536</v>
+        <v>1683332.4518800001</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>2.2853023975626014E-2</v>
+        <v>2.2344320555551727E-2</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="2"/>
-        <v>2.4815619758030535E-2</v>
+        <v>2.4717894667533394E-2</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
@@ -4477,15 +4477,15 @@
       </c>
       <c r="E23" s="2">
         <f t="shared" si="0"/>
-        <v>1971456.2500700001</v>
+        <v>1788540.7301225001</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>2.2969056951100117E-2</v>
+        <v>2.248482049816132E-2</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="2"/>
-        <v>2.483501081328501E-2</v>
+        <v>2.4746954882941218E-2</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
@@ -4495,15 +4495,15 @@
       </c>
       <c r="E24" s="2">
         <f t="shared" si="0"/>
-        <v>2087424.2647800001</v>
+        <v>1893749.0083650001</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>2.3073191033199707E-2</v>
+        <v>2.2611201007686849E-2</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="2"/>
-        <v>2.4851496288218318E-2</v>
+        <v>2.4771745574972949E-2</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
@@ -4513,15 +4513,15 @@
       </c>
       <c r="E25" s="2">
         <f t="shared" si="0"/>
-        <v>2203392.2794900001</v>
+        <v>1998957.2866075002</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>2.3167167255522449E-2</v>
+        <v>2.2725488637914373E-2</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="2"/>
-        <v>2.4865628965230833E-2</v>
+        <v>2.4793063922549739E-2</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
@@ -4531,15 +4531,15 @@
       </c>
       <c r="E26" s="2">
         <f t="shared" si="0"/>
-        <v>2319360.2941999999</v>
+        <v>2104165.5648500002</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>2.3252402785950189E-2</v>
+        <v>2.2829339823549524E-2</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="2"/>
-        <v>2.4877836159097812E-2</v>
+        <v>2.4811529375934876E-2</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
@@ -4549,15 +4549,15 @@
       </c>
       <c r="E27" s="2">
         <f t="shared" si="0"/>
-        <v>2435328.3089100001</v>
+        <v>2209373.8430925002</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>2.333006288672055E-2</v>
+        <v>2.292412168645408E-2</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="2"/>
-        <v>2.4888452401507683E-2</v>
+        <v>2.4827629169093993E-2</v>
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
@@ -4567,15 +4567,15 @@
       </c>
       <c r="E28" s="2">
         <f t="shared" si="0"/>
-        <v>2551296.3236199999</v>
+        <v>2314582.1213350003</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>2.3401114504179883E-2</v>
+        <v>2.3010972557190573E-2</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="2"/>
-        <v>2.4897742606850248E-2</v>
+        <v>2.4841750793270036E-2</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
@@ -4585,15 +4585,15 @@
       </c>
       <c r="E29" s="2">
         <f t="shared" si="0"/>
-        <v>2667264.3383300002</v>
+        <v>2419790.3995775003</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>2.3466366736204426E-2</v>
+        <v>2.309084791402315E-2</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="2"/>
-        <v>2.4905918760487197E-2</v>
+        <v>2.4854205532504413E-2</v>
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
@@ -4603,15 +4603,15 @@
       </c>
       <c r="E30" s="2">
         <f t="shared" si="0"/>
-        <v>2783232.35304</v>
+        <v>2524998.6778199999</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
-        <v>2.3526501779052925E-2</v>
+        <v>2.3164555680352937E-2</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="2"/>
-        <v>2.4913152119714635E-2</v>
+        <v>2.4865245765979017E-2</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
@@ -4621,15 +4621,15 @@
       </c>
       <c r="E31" s="2">
         <f t="shared" si="0"/>
-        <v>2899200.3677500002</v>
+        <v>2630206.9560624999</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
-        <v>2.3582098868218555E-2</v>
+        <v>2.3232783649599732E-2</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="2"/>
-        <v>2.4919582255219713E-2</v>
+        <v>2.4875077854835118E-2</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
@@ -4639,15 +4639,15 @@
       </c>
       <c r="E32" s="2">
         <f t="shared" si="0"/>
-        <v>3015168.38246</v>
+        <v>2735415.2343049999</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
-        <v>2.3633652996421256E-2</v>
+        <v>2.3296121012606478E-2</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="2"/>
-        <v>2.4925323834632456E-2</v>
+        <v>2.4883871855852759E-2</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -4657,15 +4657,15 @@
       </c>
       <c r="E33" s="2">
         <f t="shared" si="0"/>
-        <v>3131136.3971700002</v>
+        <v>2840623.5125475</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
-        <v>2.3681589691406196E-2</v>
+        <v>2.3355075415940126E-2</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="2"/>
-        <v>2.4930471770327742E-2</v>
+        <v>2.489176892451022E-2</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -4675,15 +4675,15 @@
       </c>
       <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>3247104.41188</v>
+        <v>2945831.79079</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
-        <v>2.3726276788409606E-2</v>
+        <v>2.3410086597309959E-2</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="2"/>
-        <v>2.4935105167210238E-2</v>
+        <v>2.4898887014877857E-2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -4692,15 +4692,15 @@
       </c>
       <c r="E35" s="2">
         <f t="shared" ref="E35" si="4">f*D35</f>
-        <v>2319360.2941999999</v>
+        <v>2104165.5648500002</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
-        <v>2.3252402785950189E-2</v>
+        <v>2.2829339823549524E-2</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" ref="G35" si="5">IF(D35-bmin&gt;0,p*(2*h*m*(D35-bmin)+h^2*(D35-bmin)^2)/(h*(D35-bmin)+m)^2,0)</f>
-        <v>2.4877836159097812E-2</v>
+        <v>2.4811529375934876E-2</v>
       </c>
       <c r="H35" t="s">
         <v>12</v>
@@ -4712,52 +4712,52 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>E36/f</f>
-        <v>0.50105135999999995</v>
+        <v>0.63388030000000006</v>
       </c>
       <c r="E36" s="5">
         <f>B42</f>
-        <v>116211.86297389099</v>
+        <v>133378.90994967875</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
-        <v>9.9999999719342907E-3</v>
+        <v>1.0000000386903169E-2</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" ref="G36:G37" si="6">IF(D36-bmin&gt;0,p*(2*h*m*(D36-bmin)+h^2*(D36-bmin)^2)/(h*(D36-bmin)+m)^2,0)</f>
-        <v>1.5999999966321152E-2</v>
+        <v>1.6000000464283796E-2</v>
       </c>
       <c r="H36" s="9">
         <v>0.01</v>
       </c>
       <c r="I36" s="8">
         <f>F36-H36</f>
-        <v>-2.8065709478664047E-11</v>
+        <v>3.8690316922496137E-10</v>
       </c>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" s="4">
         <f>E37/f</f>
-        <v>3.4556963500000002</v>
+        <v>2.66742334</v>
       </c>
       <c r="E37" s="5">
         <f>H42</f>
-        <v>801500.49030018668</v>
+        <v>561270.03389051743</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="1"/>
-        <v>2.0534061057964823E-2</v>
+        <v>1.8430373545949931E-2</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="6"/>
-        <v>2.4202215574640553E-2</v>
+        <v>2.3273600330169824E-2</v>
       </c>
       <c r="H37" s="9">
         <v>0.02</v>
       </c>
       <c r="I37" s="8">
         <f>F37-H37</f>
-        <v>5.3406105796482278E-4</v>
+        <v>-1.5696264540500694E-3</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -4796,92 +4796,92 @@
         <v>10</v>
       </c>
       <c r="B41" s="4">
-        <v>0.50105135999999995</v>
+        <v>0.63388029999999995</v>
       </c>
       <c r="C41" s="4">
-        <v>0.65197760999999999</v>
+        <v>0.77039457</v>
       </c>
       <c r="D41" s="4">
-        <v>0.75971648000000003</v>
+        <v>0.87985102999999998</v>
       </c>
       <c r="E41" s="4">
-        <v>0.84668591000000004</v>
+        <v>0.98640106999999999</v>
       </c>
       <c r="F41" s="7">
-        <v>0.95077845000000005</v>
+        <v>1.10487501</v>
       </c>
       <c r="G41" s="7">
-        <v>1.2536148899999999</v>
+        <v>1.52812568</v>
       </c>
       <c r="H41" s="4">
-        <v>3.4556963500000002</v>
+        <v>2.66742334</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>231936.02942000001</v>
+        <v>210416.55648500001</v>
       </c>
       <c r="B42" s="6">
         <f t="shared" ref="B42:H42" si="7">B41*sim_conv</f>
-        <v>116211.86297389099</v>
+        <v>133378.90994967875</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="7"/>
-        <v>151217.0981341413</v>
+        <v>162103.77255414228</v>
       </c>
       <c r="D42" s="6">
         <f t="shared" si="7"/>
-        <v>176205.62385613885</v>
+        <v>185135.22395238045</v>
       </c>
       <c r="E42" s="6">
         <f t="shared" si="7"/>
-        <v>196376.96813125949</v>
+        <v>207555.11646251945</v>
       </c>
       <c r="F42" s="6">
         <f t="shared" si="7"/>
-        <v>220519.778551102</v>
+        <v>232483.99495052994</v>
       </c>
       <c r="G42" s="6">
         <f t="shared" si="7"/>
-        <v>290758.46000839007</v>
+        <v>321542.94346189906</v>
       </c>
       <c r="H42" s="6">
         <f t="shared" si="7"/>
-        <v>801500.49030018668</v>
+        <v>561270.03389051743</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5">
         <f>B40*B42</f>
-        <v>29052.965743472749</v>
+        <v>33344.727487419688</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" ref="C43:H43" si="8">C40*C42</f>
-        <v>37804.274533535325</v>
+        <v>40525.943138535571</v>
       </c>
       <c r="D43" s="5">
         <f t="shared" si="8"/>
-        <v>35241.124771227769</v>
+        <v>37027.044790476088</v>
       </c>
       <c r="E43" s="5">
         <f t="shared" si="8"/>
-        <v>19637.696813125949</v>
+        <v>20755.511646251947</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="8"/>
-        <v>22051.977855110203</v>
+        <v>23248.399495052996</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="8"/>
-        <v>26168.261400755106</v>
+        <v>28938.864911570916</v>
       </c>
       <c r="H43" s="5">
         <f t="shared" si="8"/>
-        <v>8015.0049030018672</v>
+        <v>5612.7003389051742</v>
       </c>
       <c r="I43" s="5">
         <f>SUM(B43:H43)</f>
-        <v>177971.30602022895</v>
+        <v>189453.19180821237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results from latest run
</commit_message>
<xml_diff>
--- a/Data/Effective Wealth Tax Rates.xlsx
+++ b/Data/Effective Wealth Tax Rates.xlsx
@@ -360,103 +360,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-420833.11297000002</c:v>
+                  <c:v>-426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-315624.83472749998</c:v>
+                  <c:v>-320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-210416.55648500001</c:v>
+                  <c:v>-213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-105208.2782425</c:v>
+                  <c:v>-106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105208.2782425</c:v>
+                  <c:v>106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>210416.55648500001</c:v>
+                  <c:v>213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>315624.83472749998</c:v>
+                  <c:v>320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>420833.11297000002</c:v>
+                  <c:v>426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>526041.39121250005</c:v>
+                  <c:v>533453.945985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>631249.66945499997</c:v>
+                  <c:v>640144.73518200009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>736457.9476975</c:v>
+                  <c:v>746835.52437900007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>841666.22594000003</c:v>
+                  <c:v>853526.31357600004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>946874.50418250007</c:v>
+                  <c:v>960217.10277300002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1052082.7824250001</c:v>
+                  <c:v>1066907.89197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1157291.0606675001</c:v>
+                  <c:v>1173598.681167</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1262499.3389099999</c:v>
+                  <c:v>1280289.4703640002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1367707.6171525</c:v>
+                  <c:v>1386980.2595610002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1472915.895395</c:v>
+                  <c:v>1493671.0487580001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1578124.1736375</c:v>
+                  <c:v>1600361.8379550001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1683332.4518800001</c:v>
+                  <c:v>1707052.6271520001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1788540.7301225001</c:v>
+                  <c:v>1813743.4163490001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1893749.0083650001</c:v>
+                  <c:v>1920434.205546</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1998957.2866075002</c:v>
+                  <c:v>2027124.994743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2104165.5648500002</c:v>
+                  <c:v>2133815.78394</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2209373.8430925002</c:v>
+                  <c:v>2240506.5731370002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2314582.1213350003</c:v>
+                  <c:v>2347197.3623339999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2419790.3995775003</c:v>
+                  <c:v>2453888.1515310002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2524998.6778199999</c:v>
+                  <c:v>2560578.9407280004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2630206.9560624999</c:v>
+                  <c:v>2667269.7299250001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2735415.2343049999</c:v>
+                  <c:v>2773960.5191220003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2840623.5125475</c:v>
+                  <c:v>2880651.3083190001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2945831.79079</c:v>
+                  <c:v>2987342.0975160003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -483,88 +483,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6158149537096575E-3</c:v>
+                  <c:v>8.7507988122803686E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2815121343293304E-2</c:v>
+                  <c:v>1.2963839553771324E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5300998870865303E-2</c:v>
+                  <c:v>1.5442005656318215E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6944440329775812E-2</c:v>
+                  <c:v>1.7073931017184876E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8111635194022029E-2</c:v>
+                  <c:v>1.8229860043179308E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8983399046626132E-2</c:v>
+                  <c:v>1.9091542822512967E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9659297019128701E-2</c:v>
+                  <c:v>1.9758646341329275E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.0198672573236334E-2</c:v>
+                  <c:v>2.0290391941522077E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0639095031177557E-2</c:v>
+                  <c:v>2.0724182051727314E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1005507112536334E-2</c:v>
+                  <c:v>2.1084801136264108E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.131511834388209E-2</c:v>
+                  <c:v>2.1389322780800361E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1580186454555408E-2</c:v>
+                  <c:v>2.1649892020522473E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.1809678870627933E-2</c:v>
+                  <c:v>2.1875384016049555E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2010307294702967E-2</c:v>
+                  <c:v>2.2072435111922185E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2187195014935383E-2</c:v>
+                  <c:v>2.2246106902493297E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2344320555551727E-2</c:v>
+                  <c:v>2.240032716842081E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.248482049816132E-2</c:v>
+                  <c:v>2.2538190513244901E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2611201007686849E-2</c:v>
+                  <c:v>2.2662168158942956E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2725488637914373E-2</c:v>
+                  <c:v>2.2774257388583925E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.2829339823549524E-2</c:v>
+                  <c:v>2.2876089965019386E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.292412168645408E-2</c:v>
+                  <c:v>2.2969012089343478E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3010972557190573E-2</c:v>
+                  <c:v>2.3054144249819688E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.309084791402315E-2</c:v>
+                  <c:v>2.3132426624363409E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3164555680352937E-2</c:v>
+                  <c:v>2.3204653947535542E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3232783649599732E-2</c:v>
+                  <c:v>2.3271502588025666E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3296121012606478E-2</c:v>
+                  <c:v>2.3333551794007375E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3355075415940126E-2</c:v>
+                  <c:v>2.3391300521102523E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3410086597309959E-2</c:v>
+                  <c:v>2.3445180878619798E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,11 +579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="238146728"/>
-        <c:axId val="238147512"/>
+        <c:axId val="242013256"/>
+        <c:axId val="242013648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="238146728"/>
+        <c:axId val="242013256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,12 +640,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238147512"/>
+        <c:crossAx val="242013648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="238147512"/>
+        <c:axId val="242013648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238146728"/>
+        <c:crossAx val="242013256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -861,103 +861,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-420833.11297000002</c:v>
+                  <c:v>-426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-315624.83472749998</c:v>
+                  <c:v>-320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-210416.55648500001</c:v>
+                  <c:v>-213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-105208.2782425</c:v>
+                  <c:v>-106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105208.2782425</c:v>
+                  <c:v>106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>210416.55648500001</c:v>
+                  <c:v>213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>315624.83472749998</c:v>
+                  <c:v>320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>420833.11297000002</c:v>
+                  <c:v>426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>526041.39121250005</c:v>
+                  <c:v>533453.945985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>631249.66945499997</c:v>
+                  <c:v>640144.73518200009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>736457.9476975</c:v>
+                  <c:v>746835.52437900007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>841666.22594000003</c:v>
+                  <c:v>853526.31357600004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>946874.50418250007</c:v>
+                  <c:v>960217.10277300002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1052082.7824250001</c:v>
+                  <c:v>1066907.89197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1157291.0606675001</c:v>
+                  <c:v>1173598.681167</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1262499.3389099999</c:v>
+                  <c:v>1280289.4703640002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1367707.6171525</c:v>
+                  <c:v>1386980.2595610002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1472915.895395</c:v>
+                  <c:v>1493671.0487580001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1578124.1736375</c:v>
+                  <c:v>1600361.8379550001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1683332.4518800001</c:v>
+                  <c:v>1707052.6271520001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1788540.7301225001</c:v>
+                  <c:v>1813743.4163490001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1893749.0083650001</c:v>
+                  <c:v>1920434.205546</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1998957.2866075002</c:v>
+                  <c:v>2027124.994743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2104165.5648500002</c:v>
+                  <c:v>2133815.78394</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2209373.8430925002</c:v>
+                  <c:v>2240506.5731370002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2314582.1213350003</c:v>
+                  <c:v>2347197.3623339999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2419790.3995775003</c:v>
+                  <c:v>2453888.1515310002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2524998.6778199999</c:v>
+                  <c:v>2560578.9407280004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2630206.9560624999</c:v>
+                  <c:v>2667269.7299250001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2735415.2343049999</c:v>
+                  <c:v>2773960.5191220003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2840623.5125475</c:v>
+                  <c:v>2880651.3083190001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2945831.79079</c:v>
+                  <c:v>2987342.0975160003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,88 +984,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4262339214756638E-2</c:v>
+                  <c:v>1.4438538430440441E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9061149284853345E-2</c:v>
+                  <c:v>1.9205233668505618E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1237175083881756E-2</c:v>
+                  <c:v>2.1345789765045885E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2404318335978304E-2</c:v>
+                  <c:v>2.2487097219186247E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3102017211990566E-2</c:v>
+                  <c:v>2.31666081986024E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3552020518714432E-2</c:v>
+                  <c:v>2.3603605351272084E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3859075666804497E-2</c:v>
+                  <c:v>2.3901128472989568E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4077890197640284E-2</c:v>
+                  <c:v>2.4112783677420799E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4239300314115992E-2</c:v>
+                  <c:v>2.426869523492917E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4361761062880089E-2</c:v>
+                  <c:v>2.4386848714296052E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4456865887216236E-2</c:v>
+                  <c:v>2.4478520400750107E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4532195012575753E-2</c:v>
+                  <c:v>2.4551071061033644E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.4592874043659282E-2</c:v>
+                  <c:v>2.4609470998113663E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4642469501115743E-2</c:v>
+                  <c:v>2.4657174553043764E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4683525124639828E-2</c:v>
+                  <c:v>2.4696642912300198E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4717894667533394E-2</c:v>
+                  <c:v>2.4729668046749965E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4746954882941218E-2</c:v>
+                  <c:v>2.4757579762036911E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4771745574972949E-2</c:v>
+                  <c:v>2.4781381691317599E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.4793063922549739E-2</c:v>
+                  <c:v>2.4801842793109072E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4811529375934876E-2</c:v>
+                  <c:v>2.4819560246532348E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4827629169093993E-2</c:v>
+                  <c:v>2.4835003524270687E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4841750793270036E-2</c:v>
+                  <c:v>2.4848545815979617E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4854205532504413E-2</c:v>
+                  <c:v>2.4860486787464532E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4865245765979017E-2</c:v>
+                  <c:v>2.4871069302076013E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4875077854835118E-2</c:v>
+                  <c:v>2.4880491867871925E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4883871855852759E-2</c:v>
+                  <c:v>2.4888918015069761E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.489176892451022E-2</c:v>
+                  <c:v>2.4896483439463796E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4898887014877857E-2</c:v>
+                  <c:v>2.490330149999162E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,11 +1080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="238148296"/>
-        <c:axId val="196573888"/>
+        <c:axId val="242014432"/>
+        <c:axId val="242014824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="238148296"/>
+        <c:axId val="242014432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,12 +1141,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196573888"/>
+        <c:crossAx val="242014824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196573888"/>
+        <c:axId val="242014824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238148296"/>
+        <c:crossAx val="242014432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1300,103 +1300,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-420833.11297000002</c:v>
+                  <c:v>-426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-315624.83472749998</c:v>
+                  <c:v>-320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-210416.55648500001</c:v>
+                  <c:v>-213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-105208.2782425</c:v>
+                  <c:v>-106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105208.2782425</c:v>
+                  <c:v>106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>210416.55648500001</c:v>
+                  <c:v>213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>315624.83472749998</c:v>
+                  <c:v>320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>420833.11297000002</c:v>
+                  <c:v>426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>526041.39121250005</c:v>
+                  <c:v>533453.945985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>631249.66945499997</c:v>
+                  <c:v>640144.73518200009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>736457.9476975</c:v>
+                  <c:v>746835.52437900007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>841666.22594000003</c:v>
+                  <c:v>853526.31357600004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>946874.50418250007</c:v>
+                  <c:v>960217.10277300002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1052082.7824250001</c:v>
+                  <c:v>1066907.89197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1157291.0606675001</c:v>
+                  <c:v>1173598.681167</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1262499.3389099999</c:v>
+                  <c:v>1280289.4703640002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1367707.6171525</c:v>
+                  <c:v>1386980.2595610002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1472915.895395</c:v>
+                  <c:v>1493671.0487580001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1578124.1736375</c:v>
+                  <c:v>1600361.8379550001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1683332.4518800001</c:v>
+                  <c:v>1707052.6271520001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1788540.7301225001</c:v>
+                  <c:v>1813743.4163490001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1893749.0083650001</c:v>
+                  <c:v>1920434.205546</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1998957.2866075002</c:v>
+                  <c:v>2027124.994743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2104165.5648500002</c:v>
+                  <c:v>2133815.78394</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2209373.8430925002</c:v>
+                  <c:v>2240506.5731370002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2314582.1213350003</c:v>
+                  <c:v>2347197.3623339999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2419790.3995775003</c:v>
+                  <c:v>2453888.1515310002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2524998.6778199999</c:v>
+                  <c:v>2560578.9407280004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2630206.9560624999</c:v>
+                  <c:v>2667269.7299250001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2735415.2343049999</c:v>
+                  <c:v>2773960.5191220003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2840623.5125475</c:v>
+                  <c:v>2880651.3083190001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2945831.79079</c:v>
+                  <c:v>2987342.0975160003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1423,88 +1423,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6158149537096575E-3</c:v>
+                  <c:v>8.7507988122803686E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2815121343293304E-2</c:v>
+                  <c:v>1.2963839553771324E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5300998870865303E-2</c:v>
+                  <c:v>1.5442005656318215E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6944440329775812E-2</c:v>
+                  <c:v>1.7073931017184876E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8111635194022029E-2</c:v>
+                  <c:v>1.8229860043179308E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8983399046626132E-2</c:v>
+                  <c:v>1.9091542822512967E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9659297019128701E-2</c:v>
+                  <c:v>1.9758646341329275E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.0198672573236334E-2</c:v>
+                  <c:v>2.0290391941522077E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0639095031177557E-2</c:v>
+                  <c:v>2.0724182051727314E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1005507112536334E-2</c:v>
+                  <c:v>2.1084801136264108E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.131511834388209E-2</c:v>
+                  <c:v>2.1389322780800361E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1580186454555408E-2</c:v>
+                  <c:v>2.1649892020522473E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.1809678870627933E-2</c:v>
+                  <c:v>2.1875384016049555E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2010307294702967E-2</c:v>
+                  <c:v>2.2072435111922185E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2187195014935383E-2</c:v>
+                  <c:v>2.2246106902493297E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2344320555551727E-2</c:v>
+                  <c:v>2.240032716842081E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.248482049816132E-2</c:v>
+                  <c:v>2.2538190513244901E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2611201007686849E-2</c:v>
+                  <c:v>2.2662168158942956E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2725488637914373E-2</c:v>
+                  <c:v>2.2774257388583925E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.2829339823549524E-2</c:v>
+                  <c:v>2.2876089965019386E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.292412168645408E-2</c:v>
+                  <c:v>2.2969012089343478E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3010972557190573E-2</c:v>
+                  <c:v>2.3054144249819688E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.309084791402315E-2</c:v>
+                  <c:v>2.3132426624363409E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3164555680352937E-2</c:v>
+                  <c:v>2.3204653947535542E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3232783649599732E-2</c:v>
+                  <c:v>2.3271502588025666E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3296121012606478E-2</c:v>
+                  <c:v>2.3333551794007375E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3355075415940126E-2</c:v>
+                  <c:v>2.3391300521102523E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3410086597309959E-2</c:v>
+                  <c:v>2.3445180878619798E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1547,103 +1547,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-420833.11297000002</c:v>
+                  <c:v>-426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-315624.83472749998</c:v>
+                  <c:v>-320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-210416.55648500001</c:v>
+                  <c:v>-213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-105208.2782425</c:v>
+                  <c:v>-106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105208.2782425</c:v>
+                  <c:v>106690.78919700001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>210416.55648500001</c:v>
+                  <c:v>213381.57839400001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>315624.83472749998</c:v>
+                  <c:v>320072.36759100005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>420833.11297000002</c:v>
+                  <c:v>426763.15678800002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>526041.39121250005</c:v>
+                  <c:v>533453.945985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>631249.66945499997</c:v>
+                  <c:v>640144.73518200009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>736457.9476975</c:v>
+                  <c:v>746835.52437900007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>841666.22594000003</c:v>
+                  <c:v>853526.31357600004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>946874.50418250007</c:v>
+                  <c:v>960217.10277300002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1052082.7824250001</c:v>
+                  <c:v>1066907.89197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1157291.0606675001</c:v>
+                  <c:v>1173598.681167</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1262499.3389099999</c:v>
+                  <c:v>1280289.4703640002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1367707.6171525</c:v>
+                  <c:v>1386980.2595610002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1472915.895395</c:v>
+                  <c:v>1493671.0487580001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1578124.1736375</c:v>
+                  <c:v>1600361.8379550001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1683332.4518800001</c:v>
+                  <c:v>1707052.6271520001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1788540.7301225001</c:v>
+                  <c:v>1813743.4163490001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1893749.0083650001</c:v>
+                  <c:v>1920434.205546</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1998957.2866075002</c:v>
+                  <c:v>2027124.994743</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2104165.5648500002</c:v>
+                  <c:v>2133815.78394</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2209373.8430925002</c:v>
+                  <c:v>2240506.5731370002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2314582.1213350003</c:v>
+                  <c:v>2347197.3623339999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2419790.3995775003</c:v>
+                  <c:v>2453888.1515310002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2524998.6778199999</c:v>
+                  <c:v>2560578.9407280004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2630206.9560624999</c:v>
+                  <c:v>2667269.7299250001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2735415.2343049999</c:v>
+                  <c:v>2773960.5191220003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2840623.5125475</c:v>
+                  <c:v>2880651.3083190001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2945831.79079</c:v>
+                  <c:v>2987342.0975160003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,88 +1670,88 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4262339214756638E-2</c:v>
+                  <c:v>1.4438538430440441E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9061149284853345E-2</c:v>
+                  <c:v>1.9205233668505618E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1237175083881756E-2</c:v>
+                  <c:v>2.1345789765045885E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2404318335978304E-2</c:v>
+                  <c:v>2.2487097219186247E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3102017211990566E-2</c:v>
+                  <c:v>2.31666081986024E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3552020518714432E-2</c:v>
+                  <c:v>2.3603605351272084E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3859075666804497E-2</c:v>
+                  <c:v>2.3901128472989568E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4077890197640284E-2</c:v>
+                  <c:v>2.4112783677420799E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4239300314115992E-2</c:v>
+                  <c:v>2.426869523492917E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4361761062880089E-2</c:v>
+                  <c:v>2.4386848714296052E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4456865887216236E-2</c:v>
+                  <c:v>2.4478520400750107E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4532195012575753E-2</c:v>
+                  <c:v>2.4551071061033644E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.4592874043659282E-2</c:v>
+                  <c:v>2.4609470998113663E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4642469501115743E-2</c:v>
+                  <c:v>2.4657174553043764E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4683525124639828E-2</c:v>
+                  <c:v>2.4696642912300198E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4717894667533394E-2</c:v>
+                  <c:v>2.4729668046749965E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4746954882941218E-2</c:v>
+                  <c:v>2.4757579762036911E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4771745574972949E-2</c:v>
+                  <c:v>2.4781381691317599E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.4793063922549739E-2</c:v>
+                  <c:v>2.4801842793109072E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4811529375934876E-2</c:v>
+                  <c:v>2.4819560246532348E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4827629169093993E-2</c:v>
+                  <c:v>2.4835003524270687E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4841750793270036E-2</c:v>
+                  <c:v>2.4848545815979617E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4854205532504413E-2</c:v>
+                  <c:v>2.4860486787464532E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4865245765979017E-2</c:v>
+                  <c:v>2.4871069302076013E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4875077854835118E-2</c:v>
+                  <c:v>2.4880491867871925E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4883871855852759E-2</c:v>
+                  <c:v>2.4888918015069761E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.489176892451022E-2</c:v>
+                  <c:v>2.4896483439463796E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.4898887014877857E-2</c:v>
+                  <c:v>2.490330149999162E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1766,11 +1766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196574672"/>
-        <c:axId val="196575064"/>
+        <c:axId val="242015608"/>
+        <c:axId val="242016000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196574672"/>
+        <c:axId val="242015608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,12 +1827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196575064"/>
+        <c:crossAx val="242016000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196575064"/>
+        <c:axId val="242016000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,7 +1889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196574672"/>
+        <c:crossAx val="242015608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.01"/>
@@ -4047,7 +4047,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.1867121650630199</v>
+        <v>1.43837993119209</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E34" si="0">f*D2</f>
-        <v>-420833.11297000002</v>
+        <v>-426763.15678800002</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F37" si="1">IF(D2-bmin&gt;0,p*(h*D2-bmin)/(h*D2-bmin+m),0)</f>
@@ -4073,7 +4073,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.12835012204532</v>
+        <v>1.3354509335489999</v>
       </c>
       <c r="C3">
         <v>0.6</v>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
-        <v>-315624.83472749998</v>
+        <v>-320072.36759100005</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="1"/>
@@ -4100,7 +4100,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>210416.55648500001</v>
+        <v>213381.57839400001</v>
       </c>
       <c r="D4">
         <f t="shared" si="3"/>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>-210416.55648500001</v>
+        <v>-213381.57839400001</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>-105208.2782425</v>
+        <v>-106690.78919700001</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
@@ -4174,15 +4174,15 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>105208.2782425</v>
+        <v>106690.78919700001</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>8.6158149537096575E-3</v>
+        <v>8.7507988122803686E-3</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="2"/>
-        <v>1.4262339214756638E-2</v>
+        <v>1.4438538430440441E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
       </c>
       <c r="B8" s="4">
         <f>ABS(I36)+ABS(I37)</f>
-        <v>1.5696268409532387E-3</v>
+        <v>1.6661753952790133E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
@@ -4199,15 +4199,15 @@
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>210416.55648500001</v>
+        <v>213381.57839400001</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>1.2815121343293304E-2</v>
+        <v>1.2963839553771324E-2</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="2"/>
-        <v>1.9061149284853345E-2</v>
+        <v>1.9205233668505618E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4223,15 +4223,15 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>315624.83472749998</v>
+        <v>320072.36759100005</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>1.5300998870865303E-2</v>
+        <v>1.5442005656318215E-2</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="2"/>
-        <v>2.1237175083881756E-2</v>
+        <v>2.1345789765045885E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4241,15 +4241,15 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>420833.11297000002</v>
+        <v>426763.15678800002</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>1.6944440329775812E-2</v>
+        <v>1.7073931017184876E-2</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="2"/>
-        <v>2.2404318335978304E-2</v>
+        <v>2.2487097219186247E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4259,15 +4259,15 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>526041.39121250005</v>
+        <v>533453.945985</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>1.8111635194022029E-2</v>
+        <v>1.8229860043179308E-2</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="2"/>
-        <v>2.3102017211990566E-2</v>
+        <v>2.31666081986024E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4278,15 +4278,15 @@
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>631249.66945499997</v>
+        <v>640144.73518200009</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
-        <v>1.8983399046626132E-2</v>
+        <v>1.9091542822512967E-2</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="2"/>
-        <v>2.3552020518714432E-2</v>
+        <v>2.3603605351272084E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4297,15 +4297,15 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>736457.9476975</v>
+        <v>746835.52437900007</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>1.9659297019128701E-2</v>
+        <v>1.9758646341329275E-2</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="2"/>
-        <v>2.3859075666804497E-2</v>
+        <v>2.3901128472989568E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4315,15 +4315,15 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>841666.22594000003</v>
+        <v>853526.31357600004</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>2.0198672573236334E-2</v>
+        <v>2.0290391941522077E-2</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="2"/>
-        <v>2.4077890197640284E-2</v>
+        <v>2.4112783677420799E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4333,15 +4333,15 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>946874.50418250007</v>
+        <v>960217.10277300002</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>2.0639095031177557E-2</v>
+        <v>2.0724182051727314E-2</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="2"/>
-        <v>2.4239300314115992E-2</v>
+        <v>2.426869523492917E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4351,15 +4351,15 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>1052082.7824250001</v>
+        <v>1066907.89197</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>2.1005507112536334E-2</v>
+        <v>2.1084801136264108E-2</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="2"/>
-        <v>2.4361761062880089E-2</v>
+        <v>2.4386848714296052E-2</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
@@ -4369,15 +4369,15 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>1157291.0606675001</v>
+        <v>1173598.681167</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>2.131511834388209E-2</v>
+        <v>2.1389322780800361E-2</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="2"/>
-        <v>2.4456865887216236E-2</v>
+        <v>2.4478520400750107E-2</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
@@ -4387,15 +4387,15 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>1262499.3389099999</v>
+        <v>1280289.4703640002</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>2.1580186454555408E-2</v>
+        <v>2.1649892020522473E-2</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="2"/>
-        <v>2.4532195012575753E-2</v>
+        <v>2.4551071061033644E-2</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
@@ -4405,15 +4405,15 @@
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>1367707.6171525</v>
+        <v>1386980.2595610002</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>2.1809678870627933E-2</v>
+        <v>2.1875384016049555E-2</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="2"/>
-        <v>2.4592874043659282E-2</v>
+        <v>2.4609470998113663E-2</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
@@ -4423,15 +4423,15 @@
       </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>1472915.895395</v>
+        <v>1493671.0487580001</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>2.2010307294702967E-2</v>
+        <v>2.2072435111922185E-2</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="2"/>
-        <v>2.4642469501115743E-2</v>
+        <v>2.4657174553043764E-2</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
@@ -4441,15 +4441,15 @@
       </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>1578124.1736375</v>
+        <v>1600361.8379550001</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
-        <v>2.2187195014935383E-2</v>
+        <v>2.2246106902493297E-2</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="2"/>
-        <v>2.4683525124639828E-2</v>
+        <v>2.4696642912300198E-2</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
@@ -4459,15 +4459,15 @@
       </c>
       <c r="E22" s="2">
         <f t="shared" si="0"/>
-        <v>1683332.4518800001</v>
+        <v>1707052.6271520001</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
-        <v>2.2344320555551727E-2</v>
+        <v>2.240032716842081E-2</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="2"/>
-        <v>2.4717894667533394E-2</v>
+        <v>2.4729668046749965E-2</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
@@ -4477,15 +4477,15 @@
       </c>
       <c r="E23" s="2">
         <f t="shared" si="0"/>
-        <v>1788540.7301225001</v>
+        <v>1813743.4163490001</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>2.248482049816132E-2</v>
+        <v>2.2538190513244901E-2</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="2"/>
-        <v>2.4746954882941218E-2</v>
+        <v>2.4757579762036911E-2</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
@@ -4495,15 +4495,15 @@
       </c>
       <c r="E24" s="2">
         <f t="shared" si="0"/>
-        <v>1893749.0083650001</v>
+        <v>1920434.205546</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>2.2611201007686849E-2</v>
+        <v>2.2662168158942956E-2</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="2"/>
-        <v>2.4771745574972949E-2</v>
+        <v>2.4781381691317599E-2</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
@@ -4513,15 +4513,15 @@
       </c>
       <c r="E25" s="2">
         <f t="shared" si="0"/>
-        <v>1998957.2866075002</v>
+        <v>2027124.994743</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>2.2725488637914373E-2</v>
+        <v>2.2774257388583925E-2</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="2"/>
-        <v>2.4793063922549739E-2</v>
+        <v>2.4801842793109072E-2</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
@@ -4531,15 +4531,15 @@
       </c>
       <c r="E26" s="2">
         <f t="shared" si="0"/>
-        <v>2104165.5648500002</v>
+        <v>2133815.78394</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>2.2829339823549524E-2</v>
+        <v>2.2876089965019386E-2</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="2"/>
-        <v>2.4811529375934876E-2</v>
+        <v>2.4819560246532348E-2</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
@@ -4549,15 +4549,15 @@
       </c>
       <c r="E27" s="2">
         <f t="shared" si="0"/>
-        <v>2209373.8430925002</v>
+        <v>2240506.5731370002</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>2.292412168645408E-2</v>
+        <v>2.2969012089343478E-2</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="2"/>
-        <v>2.4827629169093993E-2</v>
+        <v>2.4835003524270687E-2</v>
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
@@ -4567,15 +4567,15 @@
       </c>
       <c r="E28" s="2">
         <f t="shared" si="0"/>
-        <v>2314582.1213350003</v>
+        <v>2347197.3623339999</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>2.3010972557190573E-2</v>
+        <v>2.3054144249819688E-2</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="2"/>
-        <v>2.4841750793270036E-2</v>
+        <v>2.4848545815979617E-2</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
@@ -4585,15 +4585,15 @@
       </c>
       <c r="E29" s="2">
         <f t="shared" si="0"/>
-        <v>2419790.3995775003</v>
+        <v>2453888.1515310002</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>2.309084791402315E-2</v>
+        <v>2.3132426624363409E-2</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="2"/>
-        <v>2.4854205532504413E-2</v>
+        <v>2.4860486787464532E-2</v>
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
@@ -4603,15 +4603,15 @@
       </c>
       <c r="E30" s="2">
         <f t="shared" si="0"/>
-        <v>2524998.6778199999</v>
+        <v>2560578.9407280004</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
-        <v>2.3164555680352937E-2</v>
+        <v>2.3204653947535542E-2</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="2"/>
-        <v>2.4865245765979017E-2</v>
+        <v>2.4871069302076013E-2</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
@@ -4621,15 +4621,15 @@
       </c>
       <c r="E31" s="2">
         <f t="shared" si="0"/>
-        <v>2630206.9560624999</v>
+        <v>2667269.7299250001</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
-        <v>2.3232783649599732E-2</v>
+        <v>2.3271502588025666E-2</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="2"/>
-        <v>2.4875077854835118E-2</v>
+        <v>2.4880491867871925E-2</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
@@ -4639,15 +4639,15 @@
       </c>
       <c r="E32" s="2">
         <f t="shared" si="0"/>
-        <v>2735415.2343049999</v>
+        <v>2773960.5191220003</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
-        <v>2.3296121012606478E-2</v>
+        <v>2.3333551794007375E-2</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="2"/>
-        <v>2.4883871855852759E-2</v>
+        <v>2.4888918015069761E-2</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -4657,15 +4657,15 @@
       </c>
       <c r="E33" s="2">
         <f t="shared" si="0"/>
-        <v>2840623.5125475</v>
+        <v>2880651.3083190001</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
-        <v>2.3355075415940126E-2</v>
+        <v>2.3391300521102523E-2</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="2"/>
-        <v>2.489176892451022E-2</v>
+        <v>2.4896483439463796E-2</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -4675,15 +4675,15 @@
       </c>
       <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>2945831.79079</v>
+        <v>2987342.0975160003</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
-        <v>2.3410086597309959E-2</v>
+        <v>2.3445180878619798E-2</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="2"/>
-        <v>2.4898887014877857E-2</v>
+        <v>2.490330149999162E-2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -4692,15 +4692,15 @@
       </c>
       <c r="E35" s="2">
         <f t="shared" ref="E35" si="4">f*D35</f>
-        <v>2104165.5648500002</v>
+        <v>2133815.78394</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
-        <v>2.2829339823549524E-2</v>
+        <v>2.2876089965019386E-2</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" ref="G35" si="5">IF(D35-bmin&gt;0,p*(2*h*m*(D35-bmin)+h^2*(D35-bmin)^2)/(h*(D35-bmin)+m)^2,0)</f>
-        <v>2.4811529375934876E-2</v>
+        <v>2.4819560246532348E-2</v>
       </c>
       <c r="H35" t="s">
         <v>12</v>
@@ -4712,52 +4712,52 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>E36/f</f>
-        <v>0.63388030000000006</v>
+        <v>0.61896070999999997</v>
       </c>
       <c r="E36" s="5">
         <f>B42</f>
-        <v>133378.90994967875</v>
+        <v>132074.81326367089</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
-        <v>1.0000000386903169E-2</v>
+        <v>1.0000000276947396E-2</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" ref="G36:G37" si="6">IF(D36-bmin&gt;0,p*(2*h*m*(D36-bmin)+h^2*(D36-bmin)^2)/(h*(D36-bmin)+m)^2,0)</f>
-        <v>1.6000000464283796E-2</v>
+        <v>1.600000033233687E-2</v>
       </c>
       <c r="H36" s="9">
         <v>0.01</v>
       </c>
       <c r="I36" s="8">
         <f>F36-H36</f>
-        <v>3.8690316922496137E-10</v>
+        <v>2.7694739557215797E-10</v>
       </c>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" s="4">
         <f>E37/f</f>
-        <v>2.66742334</v>
+        <v>2.55346954</v>
       </c>
       <c r="E37" s="5">
         <f>H42</f>
-        <v>561270.03389051743</v>
+        <v>544863.36082620115</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="1"/>
-        <v>1.8430373545949931E-2</v>
+        <v>1.8333824881668383E-2</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="6"/>
-        <v>2.3273600330169824E-2</v>
+        <v>2.3222484371669464E-2</v>
       </c>
       <c r="H37" s="9">
         <v>0.02</v>
       </c>
       <c r="I37" s="8">
         <f>F37-H37</f>
-        <v>-1.5696264540500694E-3</v>
+        <v>-1.6661751183316177E-3</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -4796,92 +4796,92 @@
         <v>10</v>
       </c>
       <c r="B41" s="4">
-        <v>0.63388029999999995</v>
+        <v>0.61896070999999997</v>
       </c>
       <c r="C41" s="4">
-        <v>0.77039457</v>
+        <v>0.74816643999999999</v>
       </c>
       <c r="D41" s="4">
-        <v>0.87985102999999998</v>
+        <v>0.86089705999999999</v>
       </c>
       <c r="E41" s="4">
-        <v>0.98640106999999999</v>
+        <v>0.97412798</v>
       </c>
       <c r="F41" s="7">
-        <v>1.10487501</v>
+        <v>1.0735994</v>
       </c>
       <c r="G41" s="7">
-        <v>1.52812568</v>
+        <v>1.4520608100000001</v>
       </c>
       <c r="H41" s="4">
-        <v>2.66742334</v>
+        <v>2.55346954</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>210416.55648500001</v>
+        <v>213381.57839400001</v>
       </c>
       <c r="B42" s="6">
         <f t="shared" ref="B42:H42" si="7">B41*sim_conv</f>
-        <v>133378.90994967875</v>
+        <v>132074.81326367089</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="7"/>
-        <v>162103.77255414228</v>
+        <v>159644.93586861991</v>
       </c>
       <c r="D42" s="6">
         <f t="shared" si="7"/>
-        <v>185135.22395238045</v>
+        <v>183699.57349755414</v>
       </c>
       <c r="E42" s="6">
         <f t="shared" si="7"/>
-        <v>207555.11646251945</v>
+        <v>207860.96593015888</v>
       </c>
       <c r="F42" s="6">
         <f t="shared" si="7"/>
-        <v>232483.99495052994</v>
+        <v>229086.33453485137</v>
       </c>
       <c r="G42" s="6">
         <f t="shared" si="7"/>
-        <v>321542.94346189906</v>
+        <v>309843.02756187017</v>
       </c>
       <c r="H42" s="6">
         <f t="shared" si="7"/>
-        <v>561270.03389051743</v>
+        <v>544863.36082620115</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5">
         <f>B40*B42</f>
-        <v>33344.727487419688</v>
+        <v>33018.703315917723</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" ref="C43:H43" si="8">C40*C42</f>
-        <v>40525.943138535571</v>
+        <v>39911.233967154978</v>
       </c>
       <c r="D43" s="5">
         <f t="shared" si="8"/>
-        <v>37027.044790476088</v>
+        <v>36739.914699510831</v>
       </c>
       <c r="E43" s="5">
         <f t="shared" si="8"/>
-        <v>20755.511646251947</v>
+        <v>20786.096593015889</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="8"/>
-        <v>23248.399495052996</v>
+        <v>22908.633453485138</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="8"/>
-        <v>28938.864911570916</v>
+        <v>27885.872480568316</v>
       </c>
       <c r="H43" s="5">
         <f t="shared" si="8"/>
-        <v>5612.7003389051742</v>
+        <v>5448.6336082620119</v>
       </c>
       <c r="I43" s="5">
         <f>SUM(B43:H43)</f>
-        <v>189453.19180821237</v>
+        <v>186699.08811791489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prelim results for different sigmas
</commit_message>
<xml_diff>
--- a/Data/Effective Wealth Tax Rates.xlsx
+++ b/Data/Effective Wealth Tax Rates.xlsx
@@ -360,103 +360,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-426763.15678800002</c:v>
+                  <c:v>-311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-320072.36759100005</c:v>
+                  <c:v>-233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-213381.57839400001</c:v>
+                  <c:v>-155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-106690.78919700001</c:v>
+                  <c:v>-77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106690.78919700001</c:v>
+                  <c:v>77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>213381.57839400001</c:v>
+                  <c:v>155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>320072.36759100005</c:v>
+                  <c:v>233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>426763.15678800002</c:v>
+                  <c:v>311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>533453.945985</c:v>
+                  <c:v>389201.07842999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>640144.73518200009</c:v>
+                  <c:v>467041.29411599995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>746835.52437900007</c:v>
+                  <c:v>544881.50980200002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>853526.31357600004</c:v>
+                  <c:v>622721.72548799997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>960217.10277300002</c:v>
+                  <c:v>700561.94117399992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1066907.89197</c:v>
+                  <c:v>778402.15685999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1173598.681167</c:v>
+                  <c:v>856242.37254599994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1280289.4703640002</c:v>
+                  <c:v>934082.58823199989</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1386980.2595610002</c:v>
+                  <c:v>1011922.803918</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1493671.0487580001</c:v>
+                  <c:v>1089763.019604</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1600361.8379550001</c:v>
+                  <c:v>1167603.23529</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1707052.6271520001</c:v>
+                  <c:v>1245443.4509759999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1813743.4163490001</c:v>
+                  <c:v>1323283.6666619999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1920434.205546</c:v>
+                  <c:v>1401123.8823479998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2027124.994743</c:v>
+                  <c:v>1478964.098034</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2133815.78394</c:v>
+                  <c:v>1556804.31372</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2240506.5731370002</c:v>
+                  <c:v>1634644.5294059999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2347197.3623339999</c:v>
+                  <c:v>1712484.7450919999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2453888.1515310002</c:v>
+                  <c:v>1790324.9607779998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2560578.9407280004</c:v>
+                  <c:v>1868165.1764639998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2667269.7299250001</c:v>
+                  <c:v>1946005.39215</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2773960.5191220003</c:v>
+                  <c:v>2023845.6078359999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2880651.3083190001</c:v>
+                  <c:v>2101685.8235220001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2987342.0975160003</c:v>
+                  <c:v>2179526.0392080001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,11 +579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242013256"/>
-        <c:axId val="242013648"/>
+        <c:axId val="244410984"/>
+        <c:axId val="244411376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242013256"/>
+        <c:axId val="244410984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,12 +640,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242013648"/>
+        <c:crossAx val="244411376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242013648"/>
+        <c:axId val="244411376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242013256"/>
+        <c:crossAx val="244410984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -861,103 +861,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-426763.15678800002</c:v>
+                  <c:v>-311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-320072.36759100005</c:v>
+                  <c:v>-233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-213381.57839400001</c:v>
+                  <c:v>-155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-106690.78919700001</c:v>
+                  <c:v>-77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106690.78919700001</c:v>
+                  <c:v>77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>213381.57839400001</c:v>
+                  <c:v>155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>320072.36759100005</c:v>
+                  <c:v>233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>426763.15678800002</c:v>
+                  <c:v>311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>533453.945985</c:v>
+                  <c:v>389201.07842999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>640144.73518200009</c:v>
+                  <c:v>467041.29411599995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>746835.52437900007</c:v>
+                  <c:v>544881.50980200002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>853526.31357600004</c:v>
+                  <c:v>622721.72548799997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>960217.10277300002</c:v>
+                  <c:v>700561.94117399992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1066907.89197</c:v>
+                  <c:v>778402.15685999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1173598.681167</c:v>
+                  <c:v>856242.37254599994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1280289.4703640002</c:v>
+                  <c:v>934082.58823199989</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1386980.2595610002</c:v>
+                  <c:v>1011922.803918</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1493671.0487580001</c:v>
+                  <c:v>1089763.019604</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1600361.8379550001</c:v>
+                  <c:v>1167603.23529</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1707052.6271520001</c:v>
+                  <c:v>1245443.4509759999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1813743.4163490001</c:v>
+                  <c:v>1323283.6666619999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1920434.205546</c:v>
+                  <c:v>1401123.8823479998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2027124.994743</c:v>
+                  <c:v>1478964.098034</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2133815.78394</c:v>
+                  <c:v>1556804.31372</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2240506.5731370002</c:v>
+                  <c:v>1634644.5294059999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2347197.3623339999</c:v>
+                  <c:v>1712484.7450919999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2453888.1515310002</c:v>
+                  <c:v>1790324.9607779998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2560578.9407280004</c:v>
+                  <c:v>1868165.1764639998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2667269.7299250001</c:v>
+                  <c:v>1946005.39215</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2773960.5191220003</c:v>
+                  <c:v>2023845.6078359999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2880651.3083190001</c:v>
+                  <c:v>2101685.8235220001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2987342.0975160003</c:v>
+                  <c:v>2179526.0392080001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,11 +1080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242014432"/>
-        <c:axId val="242014824"/>
+        <c:axId val="244412160"/>
+        <c:axId val="244412552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242014432"/>
+        <c:axId val="244412160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,12 +1141,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242014824"/>
+        <c:crossAx val="244412552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242014824"/>
+        <c:axId val="244412552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242014432"/>
+        <c:crossAx val="244412160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1300,103 +1300,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-426763.15678800002</c:v>
+                  <c:v>-311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-320072.36759100005</c:v>
+                  <c:v>-233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-213381.57839400001</c:v>
+                  <c:v>-155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-106690.78919700001</c:v>
+                  <c:v>-77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106690.78919700001</c:v>
+                  <c:v>77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>213381.57839400001</c:v>
+                  <c:v>155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>320072.36759100005</c:v>
+                  <c:v>233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>426763.15678800002</c:v>
+                  <c:v>311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>533453.945985</c:v>
+                  <c:v>389201.07842999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>640144.73518200009</c:v>
+                  <c:v>467041.29411599995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>746835.52437900007</c:v>
+                  <c:v>544881.50980200002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>853526.31357600004</c:v>
+                  <c:v>622721.72548799997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>960217.10277300002</c:v>
+                  <c:v>700561.94117399992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1066907.89197</c:v>
+                  <c:v>778402.15685999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1173598.681167</c:v>
+                  <c:v>856242.37254599994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1280289.4703640002</c:v>
+                  <c:v>934082.58823199989</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1386980.2595610002</c:v>
+                  <c:v>1011922.803918</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1493671.0487580001</c:v>
+                  <c:v>1089763.019604</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1600361.8379550001</c:v>
+                  <c:v>1167603.23529</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1707052.6271520001</c:v>
+                  <c:v>1245443.4509759999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1813743.4163490001</c:v>
+                  <c:v>1323283.6666619999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1920434.205546</c:v>
+                  <c:v>1401123.8823479998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2027124.994743</c:v>
+                  <c:v>1478964.098034</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2133815.78394</c:v>
+                  <c:v>1556804.31372</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2240506.5731370002</c:v>
+                  <c:v>1634644.5294059999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2347197.3623339999</c:v>
+                  <c:v>1712484.7450919999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2453888.1515310002</c:v>
+                  <c:v>1790324.9607779998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2560578.9407280004</c:v>
+                  <c:v>1868165.1764639998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2667269.7299250001</c:v>
+                  <c:v>1946005.39215</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2773960.5191220003</c:v>
+                  <c:v>2023845.6078359999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2880651.3083190001</c:v>
+                  <c:v>2101685.8235220001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2987342.0975160003</c:v>
+                  <c:v>2179526.0392080001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1547,103 +1547,103 @@
                 <c:formatCode>"$"#,##0_)</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>-426763.15678800002</c:v>
+                  <c:v>-311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-320072.36759100005</c:v>
+                  <c:v>-233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-213381.57839400001</c:v>
+                  <c:v>-155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-106690.78919700001</c:v>
+                  <c:v>-77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106690.78919700001</c:v>
+                  <c:v>77840.215685999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>213381.57839400001</c:v>
+                  <c:v>155680.43137199999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>320072.36759100005</c:v>
+                  <c:v>233520.64705799997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>426763.15678800002</c:v>
+                  <c:v>311360.86274399998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>533453.945985</c:v>
+                  <c:v>389201.07842999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>640144.73518200009</c:v>
+                  <c:v>467041.29411599995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>746835.52437900007</c:v>
+                  <c:v>544881.50980200002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>853526.31357600004</c:v>
+                  <c:v>622721.72548799997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>960217.10277300002</c:v>
+                  <c:v>700561.94117399992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1066907.89197</c:v>
+                  <c:v>778402.15685999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1173598.681167</c:v>
+                  <c:v>856242.37254599994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1280289.4703640002</c:v>
+                  <c:v>934082.58823199989</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1386980.2595610002</c:v>
+                  <c:v>1011922.803918</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1493671.0487580001</c:v>
+                  <c:v>1089763.019604</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1600361.8379550001</c:v>
+                  <c:v>1167603.23529</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1707052.6271520001</c:v>
+                  <c:v>1245443.4509759999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1813743.4163490001</c:v>
+                  <c:v>1323283.6666619999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1920434.205546</c:v>
+                  <c:v>1401123.8823479998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2027124.994743</c:v>
+                  <c:v>1478964.098034</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2133815.78394</c:v>
+                  <c:v>1556804.31372</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2240506.5731370002</c:v>
+                  <c:v>1634644.5294059999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2347197.3623339999</c:v>
+                  <c:v>1712484.7450919999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2453888.1515310002</c:v>
+                  <c:v>1790324.9607779998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2560578.9407280004</c:v>
+                  <c:v>1868165.1764639998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2667269.7299250001</c:v>
+                  <c:v>1946005.39215</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2773960.5191220003</c:v>
+                  <c:v>2023845.6078359999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2880651.3083190001</c:v>
+                  <c:v>2101685.8235220001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2987342.0975160003</c:v>
+                  <c:v>2179526.0392080001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1766,11 +1766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242015608"/>
-        <c:axId val="242016000"/>
+        <c:axId val="244413336"/>
+        <c:axId val="244413728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242015608"/>
+        <c:axId val="244413336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,12 +1827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242016000"/>
+        <c:crossAx val="244413728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242016000"/>
+        <c:axId val="244413728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,7 +1889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242015608"/>
+        <c:crossAx val="244413336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.01"/>
@@ -4016,8 +4016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E34" si="0">f*D2</f>
-        <v>-426763.15678800002</v>
+        <v>-311360.86274399998</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F37" si="1">IF(D2-bmin&gt;0,p*(h*D2-bmin)/(h*D2-bmin+m),0)</f>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
-        <v>-320072.36759100005</v>
+        <v>-233520.64705799997</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="1"/>
@@ -4100,7 +4100,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>213381.57839400001</v>
+        <v>155680.43137199999</v>
       </c>
       <c r="D4">
         <f t="shared" si="3"/>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>-213381.57839400001</v>
+        <v>-155680.43137199999</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>-106690.78919700001</v>
+        <v>-77840.215685999996</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>106690.78919700001</v>
+        <v>77840.215685999996</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="B8" s="4">
         <f>ABS(I36)+ABS(I37)</f>
-        <v>1.6661753952790133E-3</v>
+        <v>8.7091734365588435E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>213381.57839400001</v>
+        <v>155680.43137199999</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>320072.36759100005</v>
+        <v>233520.64705799997</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>426763.15678800002</v>
+        <v>311360.86274399998</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>533453.945985</v>
+        <v>389201.07842999999</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>640144.73518200009</v>
+        <v>467041.29411599995</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="1"/>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>746835.52437900007</v>
+        <v>544881.50980200002</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>853526.31357600004</v>
+        <v>622721.72548799997</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>960217.10277300002</v>
+        <v>700561.94117399992</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>1066907.89197</v>
+        <v>778402.15685999999</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>1173598.681167</v>
+        <v>856242.37254599994</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>1280289.4703640002</v>
+        <v>934082.58823199989</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>1386980.2595610002</v>
+        <v>1011922.803918</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>1493671.0487580001</v>
+        <v>1089763.019604</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>1600361.8379550001</v>
+        <v>1167603.23529</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="1"/>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="E22" s="2">
         <f t="shared" si="0"/>
-        <v>1707052.6271520001</v>
+        <v>1245443.4509759999</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="1"/>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="E23" s="2">
         <f t="shared" si="0"/>
-        <v>1813743.4163490001</v>
+        <v>1323283.6666619999</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
@@ -4495,7 +4495,7 @@
       </c>
       <c r="E24" s="2">
         <f t="shared" si="0"/>
-        <v>1920434.205546</v>
+        <v>1401123.8823479998</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="E25" s="2">
         <f t="shared" si="0"/>
-        <v>2027124.994743</v>
+        <v>1478964.098034</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="E26" s="2">
         <f t="shared" si="0"/>
-        <v>2133815.78394</v>
+        <v>1556804.31372</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="E27" s="2">
         <f t="shared" si="0"/>
-        <v>2240506.5731370002</v>
+        <v>1634644.5294059999</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
@@ -4567,7 +4567,7 @@
       </c>
       <c r="E28" s="2">
         <f t="shared" si="0"/>
-        <v>2347197.3623339999</v>
+        <v>1712484.7450919999</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="E29" s="2">
         <f t="shared" si="0"/>
-        <v>2453888.1515310002</v>
+        <v>1790324.9607779998</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="E30" s="2">
         <f t="shared" si="0"/>
-        <v>2560578.9407280004</v>
+        <v>1868165.1764639998</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="E31" s="2">
         <f t="shared" si="0"/>
-        <v>2667269.7299250001</v>
+        <v>1946005.39215</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="E32" s="2">
         <f t="shared" si="0"/>
-        <v>2773960.5191220003</v>
+        <v>2023845.6078359999</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="E33" s="2">
         <f t="shared" si="0"/>
-        <v>2880651.3083190001</v>
+        <v>2101685.8235220001</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>2987342.0975160003</v>
+        <v>2179526.0392080001</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="E35" s="2">
         <f t="shared" ref="E35" si="4">f*D35</f>
-        <v>2133815.78394</v>
+        <v>1556804.31372</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
@@ -4712,52 +4712,52 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
         <f>E36/f</f>
-        <v>0.61896070999999997</v>
+        <v>1.5747536799999999</v>
       </c>
       <c r="E36" s="5">
         <f>B42</f>
-        <v>132074.81326367089</v>
+        <v>245158.33220704441</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
-        <v>1.0000000276947396E-2</v>
+        <v>1.572743900674721E-2</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" ref="G36:G37" si="6">IF(D36-bmin&gt;0,p*(2*h*m*(D36-bmin)+h^2*(D36-bmin)^2)/(h*(D36-bmin)+m)^2,0)</f>
-        <v>1.600000033233687E-2</v>
+        <v>2.1560784505056271E-2</v>
       </c>
       <c r="H36" s="9">
         <v>0.01</v>
       </c>
       <c r="I36" s="8">
         <f>F36-H36</f>
-        <v>2.7694739557215797E-10</v>
+        <v>5.7274390067472095E-3</v>
       </c>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" s="4">
         <f>E37/f</f>
-        <v>2.55346954</v>
+        <v>10.57204033</v>
       </c>
       <c r="E37" s="5">
         <f>H42</f>
-        <v>544863.36082620115</v>
+        <v>1645859.7990565812</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="1"/>
-        <v>1.8333824881668383E-2</v>
+        <v>2.2981734429811634E-2</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="6"/>
-        <v>2.3222484371669464E-2</v>
+        <v>2.4837064163527687E-2</v>
       </c>
       <c r="H37" s="9">
         <v>0.02</v>
       </c>
       <c r="I37" s="8">
         <f>F37-H37</f>
-        <v>-1.6661751183316177E-3</v>
+        <v>2.981734429811634E-3</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -4796,92 +4796,92 @@
         <v>10</v>
       </c>
       <c r="B41" s="4">
-        <v>0.61896070999999997</v>
+        <v>1.5747536799999999</v>
       </c>
       <c r="C41" s="4">
-        <v>0.74816643999999999</v>
+        <v>2.0575342000000001</v>
       </c>
       <c r="D41" s="4">
-        <v>0.86089705999999999</v>
+        <v>2.6258807000000002</v>
       </c>
       <c r="E41" s="4">
-        <v>0.97412798</v>
+        <v>3.14089441</v>
       </c>
       <c r="F41" s="7">
-        <v>1.0735994</v>
+        <v>3.6407742399999998</v>
       </c>
       <c r="G41" s="7">
-        <v>1.4520608100000001</v>
+        <v>5.1078768099999996</v>
       </c>
       <c r="H41" s="4">
-        <v>2.55346954</v>
+        <v>10.57204033</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>213381.57839400001</v>
+        <v>155680.43137199999</v>
       </c>
       <c r="B42" s="6">
         <f t="shared" ref="B42:H42" si="7">B41*sim_conv</f>
-        <v>132074.81326367089</v>
+        <v>245158.33220704441</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="7"/>
-        <v>159644.93586861991</v>
+        <v>320317.81181864289</v>
       </c>
       <c r="D42" s="6">
         <f t="shared" si="7"/>
-        <v>183699.57349755414</v>
+        <v>408798.24010740931</v>
       </c>
       <c r="E42" s="6">
         <f t="shared" si="7"/>
-        <v>207860.96593015888</v>
+        <v>488975.79664270341</v>
       </c>
       <c r="F42" s="6">
         <f t="shared" si="7"/>
-        <v>229086.33453485137</v>
+        <v>566797.30421126541</v>
       </c>
       <c r="G42" s="6">
         <f t="shared" si="7"/>
-        <v>309843.02756187017</v>
+        <v>795196.46517583518</v>
       </c>
       <c r="H42" s="6">
         <f t="shared" si="7"/>
-        <v>544863.36082620115</v>
+        <v>1645859.7990565812</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5">
         <f>B40*B42</f>
-        <v>33018.703315917723</v>
+        <v>61289.583051761103</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" ref="C43:H43" si="8">C40*C42</f>
-        <v>39911.233967154978</v>
+        <v>80079.452954660723</v>
       </c>
       <c r="D43" s="5">
         <f t="shared" si="8"/>
-        <v>36739.914699510831</v>
+        <v>81759.648021481873</v>
       </c>
       <c r="E43" s="5">
         <f t="shared" si="8"/>
-        <v>20786.096593015889</v>
+        <v>48897.579664270343</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="8"/>
-        <v>22908.633453485138</v>
+        <v>56679.730421126544</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="8"/>
-        <v>27885.872480568316</v>
+        <v>71567.681865825158</v>
       </c>
       <c r="H43" s="5">
         <f t="shared" si="8"/>
-        <v>5448.6336082620119</v>
+        <v>16458.597990565813</v>
       </c>
       <c r="I43" s="5">
         <f>SUM(B43:H43)</f>
-        <v>186699.08811791489</v>
+        <v>416732.27396969154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>